<commit_message>
made changes for step defs to work
</commit_message>
<xml_diff>
--- a/src/test/resources/swagger-testData.xlsx
+++ b/src/test/resources/swagger-testData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
   <si>
     <t>scenario</t>
   </si>
@@ -29,19 +29,25 @@
     <t>endpoint</t>
   </si>
   <si>
+    <t>allUsers</t>
+  </si>
+  <si>
+    <t>Found</t>
+  </si>
+  <si>
+    <t>/users</t>
+  </si>
+  <si>
     <t>validUserId</t>
   </si>
   <si>
-    <t>Found</t>
-  </si>
-  <si>
-    <t>/user</t>
+    <t>/user/{userId}</t>
   </si>
   <si>
     <t>validUserFirstname</t>
   </si>
   <si>
-    <t>/users/username</t>
+    <t>/users/username/{firstName}</t>
   </si>
   <si>
     <t>invalidUserId</t>
@@ -50,9 +56,15 @@
     <t>Not Found</t>
   </si>
   <si>
+    <t>/user/34343434</t>
+  </si>
+  <si>
     <t>invalidUserFirstname</t>
   </si>
   <si>
+    <t>/users/username/34343434</t>
+  </si>
+  <si>
     <t>invalidEndpoint</t>
   </si>
   <si>
@@ -131,6 +143,9 @@
     <t>july</t>
   </si>
   <si>
+    <t>Numpy@gmail.com</t>
+  </si>
+  <si>
     <t>k-89</t>
   </si>
   <si>
@@ -149,13 +164,16 @@
     <t>invalidFirstname</t>
   </si>
   <si>
+    <t>septe5mber+-</t>
+  </si>
+  <si>
     <t>k-91</t>
   </si>
   <si>
     <t>invalidLastname</t>
   </si>
   <si>
-    <t>sep</t>
+    <t>october</t>
   </si>
   <si>
     <t>k-92</t>
@@ -164,7 +182,7 @@
     <t>invalidContactNo</t>
   </si>
   <si>
-    <t>oct</t>
+    <t>november</t>
   </si>
   <si>
     <t>k-93</t>
@@ -173,13 +191,19 @@
     <t>invalidEmailId</t>
   </si>
   <si>
-    <t>nov</t>
+    <t>december</t>
+  </si>
+  <si>
+    <t>Team09Sandhya3--gmail--com</t>
   </si>
   <si>
     <t>k-94</t>
   </si>
   <si>
-    <t>/deleteuser</t>
+    <t>/deleteuser/{userId}</t>
+  </si>
+  <si>
+    <t>/deleteuser/343434434</t>
   </si>
   <si>
     <t>/deleteusers</t>
@@ -240,13 +264,13 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,7 +505,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.88"/>
-    <col customWidth="1" min="4" max="4" width="14.88"/>
+    <col customWidth="1" min="4" max="4" width="27.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -531,13 +555,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="1">
-        <v>404.0</v>
+        <v>200.0</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -548,24 +572,38 @@
         <v>404.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>404.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>404.0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -584,44 +622,44 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="14.88"/>
-    <col customWidth="1" min="3" max="3" width="8.13"/>
-    <col customWidth="1" min="4" max="4" width="10.5"/>
-    <col customWidth="1" min="5" max="5" width="17.0"/>
+    <col customWidth="1" min="4" max="4" width="15.63"/>
+    <col customWidth="1" min="5" max="5" width="20.75"/>
+    <col customWidth="1" min="6" max="6" width="17.0"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>3</v>
@@ -629,3266 +667,3271 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="B2" s="1">
+        <v>201.0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="5">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="5">
         <v>3.456789015E9</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>27</v>
+      <c r="F2" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="5">
+        <v>33</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="5">
         <v>94530.0</v>
       </c>
-      <c r="K2" s="1">
-        <v>201.0</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1">
+        <v>409.0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1.234567891E9</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="5">
-        <v>3.456789015E9</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="J3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="K3" s="5">
+        <v>94530.0</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="5">
-        <v>94530.0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>409.0</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B4" s="1">
+        <v>409.0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2.234560901E9</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>28</v>
+        <v>41</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.234560221E9</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="5">
+        <v>33</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="5">
         <v>94530.0</v>
       </c>
-      <c r="K4" s="1">
-        <v>409.0</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="B5" s="1">
+        <v>201.0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="1">
+        <v>45</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1">
         <v>2.234560901E9</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>28</v>
+      <c r="F5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="5">
+        <v>33</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="5">
         <v>94530.0</v>
       </c>
-      <c r="K5" s="1">
-        <v>201.0</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B6" s="1">
-        <v>1234.0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>28</v>
+        <v>400.0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.234560901E9</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="5">
+        <v>33</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="5">
         <v>94530.0</v>
       </c>
-      <c r="K6" s="1">
-        <v>400.0</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="1">
+        <v>400.0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.234560901E9</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="1">
-        <v>1234.0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2.234560901E9</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>28</v>
+      <c r="G7" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="5">
+        <v>33</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="5">
         <v>94530.0</v>
       </c>
-      <c r="K7" s="1">
-        <v>400.0</v>
-      </c>
       <c r="L7" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="1">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1">
+        <v>400.0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1">
         <v>12.0</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>28</v>
+      <c r="F8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="5">
+        <v>33</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="5">
         <v>94530.0</v>
       </c>
-      <c r="K8" s="1">
-        <v>400.0</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1">
+        <v>57</v>
+      </c>
+      <c r="B9" s="1">
+        <v>400.0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1">
         <v>2.234560901E9</v>
       </c>
-      <c r="E9" s="8">
-        <v>12.0</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>28</v>
+      <c r="F9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="5">
+        <v>33</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="5">
         <v>94530.0</v>
       </c>
-      <c r="K9" s="1">
-        <v>400.0</v>
-      </c>
       <c r="L9" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
-      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11">
-      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12">
-      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13">
-      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14">
-      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15">
-      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16">
-      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="17">
-      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18">
-      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
     </row>
     <row r="19">
-      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20">
-      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21">
-      <c r="E21" s="7"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22">
-      <c r="E22" s="7"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23">
-      <c r="E23" s="7"/>
+      <c r="F23" s="8"/>
     </row>
     <row r="24">
-      <c r="E24" s="7"/>
+      <c r="F24" s="8"/>
     </row>
     <row r="25">
-      <c r="E25" s="7"/>
+      <c r="F25" s="8"/>
     </row>
     <row r="26">
-      <c r="E26" s="7"/>
+      <c r="F26" s="8"/>
     </row>
     <row r="27">
-      <c r="E27" s="7"/>
+      <c r="F27" s="8"/>
     </row>
     <row r="28">
-      <c r="E28" s="7"/>
+      <c r="F28" s="8"/>
     </row>
     <row r="29">
-      <c r="E29" s="7"/>
+      <c r="F29" s="8"/>
     </row>
     <row r="30">
-      <c r="E30" s="7"/>
+      <c r="F30" s="8"/>
     </row>
     <row r="31">
-      <c r="E31" s="7"/>
+      <c r="F31" s="8"/>
     </row>
     <row r="32">
-      <c r="E32" s="7"/>
+      <c r="F32" s="8"/>
     </row>
     <row r="33">
-      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
     </row>
     <row r="34">
-      <c r="E34" s="7"/>
+      <c r="F34" s="8"/>
     </row>
     <row r="35">
-      <c r="E35" s="7"/>
+      <c r="F35" s="8"/>
     </row>
     <row r="36">
-      <c r="E36" s="7"/>
+      <c r="F36" s="8"/>
     </row>
     <row r="37">
-      <c r="E37" s="7"/>
+      <c r="F37" s="8"/>
     </row>
     <row r="38">
-      <c r="E38" s="7"/>
+      <c r="F38" s="8"/>
     </row>
     <row r="39">
-      <c r="E39" s="7"/>
+      <c r="F39" s="8"/>
     </row>
     <row r="40">
-      <c r="E40" s="7"/>
+      <c r="F40" s="8"/>
     </row>
     <row r="41">
-      <c r="E41" s="7"/>
+      <c r="F41" s="8"/>
     </row>
     <row r="42">
-      <c r="E42" s="7"/>
+      <c r="F42" s="8"/>
     </row>
     <row r="43">
-      <c r="E43" s="7"/>
+      <c r="F43" s="8"/>
     </row>
     <row r="44">
-      <c r="E44" s="7"/>
+      <c r="F44" s="8"/>
     </row>
     <row r="45">
-      <c r="E45" s="7"/>
+      <c r="F45" s="8"/>
     </row>
     <row r="46">
-      <c r="E46" s="7"/>
+      <c r="F46" s="8"/>
     </row>
     <row r="47">
-      <c r="E47" s="7"/>
+      <c r="F47" s="8"/>
     </row>
     <row r="48">
-      <c r="E48" s="7"/>
+      <c r="F48" s="8"/>
     </row>
     <row r="49">
-      <c r="E49" s="7"/>
+      <c r="F49" s="8"/>
     </row>
     <row r="50">
-      <c r="E50" s="7"/>
+      <c r="F50" s="8"/>
     </row>
     <row r="51">
-      <c r="E51" s="7"/>
+      <c r="F51" s="8"/>
     </row>
     <row r="52">
-      <c r="E52" s="7"/>
+      <c r="F52" s="8"/>
     </row>
     <row r="53">
-      <c r="E53" s="7"/>
+      <c r="F53" s="8"/>
     </row>
     <row r="54">
-      <c r="E54" s="7"/>
+      <c r="F54" s="8"/>
     </row>
     <row r="55">
-      <c r="E55" s="7"/>
+      <c r="F55" s="8"/>
     </row>
     <row r="56">
-      <c r="E56" s="7"/>
+      <c r="F56" s="8"/>
     </row>
     <row r="57">
-      <c r="E57" s="7"/>
+      <c r="F57" s="8"/>
     </row>
     <row r="58">
-      <c r="E58" s="7"/>
+      <c r="F58" s="8"/>
     </row>
     <row r="59">
-      <c r="E59" s="7"/>
+      <c r="F59" s="8"/>
     </row>
     <row r="60">
-      <c r="E60" s="7"/>
+      <c r="F60" s="8"/>
     </row>
     <row r="61">
-      <c r="E61" s="7"/>
+      <c r="F61" s="8"/>
     </row>
     <row r="62">
-      <c r="E62" s="7"/>
+      <c r="F62" s="8"/>
     </row>
     <row r="63">
-      <c r="E63" s="7"/>
+      <c r="F63" s="8"/>
     </row>
     <row r="64">
-      <c r="E64" s="7"/>
+      <c r="F64" s="8"/>
     </row>
     <row r="65">
-      <c r="E65" s="7"/>
+      <c r="F65" s="8"/>
     </row>
     <row r="66">
-      <c r="E66" s="7"/>
+      <c r="F66" s="8"/>
     </row>
     <row r="67">
-      <c r="E67" s="7"/>
+      <c r="F67" s="8"/>
     </row>
     <row r="68">
-      <c r="E68" s="7"/>
+      <c r="F68" s="8"/>
     </row>
     <row r="69">
-      <c r="E69" s="7"/>
+      <c r="F69" s="8"/>
     </row>
     <row r="70">
-      <c r="E70" s="7"/>
+      <c r="F70" s="8"/>
     </row>
     <row r="71">
-      <c r="E71" s="7"/>
+      <c r="F71" s="8"/>
     </row>
     <row r="72">
-      <c r="E72" s="7"/>
+      <c r="F72" s="8"/>
     </row>
     <row r="73">
-      <c r="E73" s="7"/>
+      <c r="F73" s="8"/>
     </row>
     <row r="74">
-      <c r="E74" s="7"/>
+      <c r="F74" s="8"/>
     </row>
     <row r="75">
-      <c r="E75" s="7"/>
+      <c r="F75" s="8"/>
     </row>
     <row r="76">
-      <c r="E76" s="7"/>
+      <c r="F76" s="8"/>
     </row>
     <row r="77">
-      <c r="E77" s="7"/>
+      <c r="F77" s="8"/>
     </row>
     <row r="78">
-      <c r="E78" s="7"/>
+      <c r="F78" s="8"/>
     </row>
     <row r="79">
-      <c r="E79" s="7"/>
+      <c r="F79" s="8"/>
     </row>
     <row r="80">
-      <c r="E80" s="7"/>
+      <c r="F80" s="8"/>
     </row>
     <row r="81">
-      <c r="E81" s="7"/>
+      <c r="F81" s="8"/>
     </row>
     <row r="82">
-      <c r="E82" s="7"/>
+      <c r="F82" s="8"/>
     </row>
     <row r="83">
-      <c r="E83" s="7"/>
+      <c r="F83" s="8"/>
     </row>
     <row r="84">
-      <c r="E84" s="7"/>
+      <c r="F84" s="8"/>
     </row>
     <row r="85">
-      <c r="E85" s="7"/>
+      <c r="F85" s="8"/>
     </row>
     <row r="86">
-      <c r="E86" s="7"/>
+      <c r="F86" s="8"/>
     </row>
     <row r="87">
-      <c r="E87" s="7"/>
+      <c r="F87" s="8"/>
     </row>
     <row r="88">
-      <c r="E88" s="7"/>
+      <c r="F88" s="8"/>
     </row>
     <row r="89">
-      <c r="E89" s="7"/>
+      <c r="F89" s="8"/>
     </row>
     <row r="90">
-      <c r="E90" s="7"/>
+      <c r="F90" s="8"/>
     </row>
     <row r="91">
-      <c r="E91" s="7"/>
+      <c r="F91" s="8"/>
     </row>
     <row r="92">
-      <c r="E92" s="7"/>
+      <c r="F92" s="8"/>
     </row>
     <row r="93">
-      <c r="E93" s="7"/>
+      <c r="F93" s="8"/>
     </row>
     <row r="94">
-      <c r="E94" s="7"/>
+      <c r="F94" s="8"/>
     </row>
     <row r="95">
-      <c r="E95" s="7"/>
+      <c r="F95" s="8"/>
     </row>
     <row r="96">
-      <c r="E96" s="7"/>
+      <c r="F96" s="8"/>
     </row>
     <row r="97">
-      <c r="E97" s="7"/>
+      <c r="F97" s="8"/>
     </row>
     <row r="98">
-      <c r="E98" s="7"/>
+      <c r="F98" s="8"/>
     </row>
     <row r="99">
-      <c r="E99" s="7"/>
+      <c r="F99" s="8"/>
     </row>
     <row r="100">
-      <c r="E100" s="7"/>
+      <c r="F100" s="8"/>
     </row>
     <row r="101">
-      <c r="E101" s="7"/>
+      <c r="F101" s="8"/>
     </row>
     <row r="102">
-      <c r="E102" s="7"/>
+      <c r="F102" s="8"/>
     </row>
     <row r="103">
-      <c r="E103" s="7"/>
+      <c r="F103" s="8"/>
     </row>
     <row r="104">
-      <c r="E104" s="7"/>
+      <c r="F104" s="8"/>
     </row>
     <row r="105">
-      <c r="E105" s="7"/>
+      <c r="F105" s="8"/>
     </row>
     <row r="106">
-      <c r="E106" s="7"/>
+      <c r="F106" s="8"/>
     </row>
     <row r="107">
-      <c r="E107" s="7"/>
+      <c r="F107" s="8"/>
     </row>
     <row r="108">
-      <c r="E108" s="7"/>
+      <c r="F108" s="8"/>
     </row>
     <row r="109">
-      <c r="E109" s="7"/>
+      <c r="F109" s="8"/>
     </row>
     <row r="110">
-      <c r="E110" s="7"/>
+      <c r="F110" s="8"/>
     </row>
     <row r="111">
-      <c r="E111" s="7"/>
+      <c r="F111" s="8"/>
     </row>
     <row r="112">
-      <c r="E112" s="7"/>
+      <c r="F112" s="8"/>
     </row>
     <row r="113">
-      <c r="E113" s="7"/>
+      <c r="F113" s="8"/>
     </row>
     <row r="114">
-      <c r="E114" s="7"/>
+      <c r="F114" s="8"/>
     </row>
     <row r="115">
-      <c r="E115" s="7"/>
+      <c r="F115" s="8"/>
     </row>
     <row r="116">
-      <c r="E116" s="7"/>
+      <c r="F116" s="8"/>
     </row>
     <row r="117">
-      <c r="E117" s="7"/>
+      <c r="F117" s="8"/>
     </row>
     <row r="118">
-      <c r="E118" s="7"/>
+      <c r="F118" s="8"/>
     </row>
     <row r="119">
-      <c r="E119" s="7"/>
+      <c r="F119" s="8"/>
     </row>
     <row r="120">
-      <c r="E120" s="7"/>
+      <c r="F120" s="8"/>
     </row>
     <row r="121">
-      <c r="E121" s="7"/>
+      <c r="F121" s="8"/>
     </row>
     <row r="122">
-      <c r="E122" s="7"/>
+      <c r="F122" s="8"/>
     </row>
     <row r="123">
-      <c r="E123" s="7"/>
+      <c r="F123" s="8"/>
     </row>
     <row r="124">
-      <c r="E124" s="7"/>
+      <c r="F124" s="8"/>
     </row>
     <row r="125">
-      <c r="E125" s="7"/>
+      <c r="F125" s="8"/>
     </row>
     <row r="126">
-      <c r="E126" s="7"/>
+      <c r="F126" s="8"/>
     </row>
     <row r="127">
-      <c r="E127" s="7"/>
+      <c r="F127" s="8"/>
     </row>
     <row r="128">
-      <c r="E128" s="7"/>
+      <c r="F128" s="8"/>
     </row>
     <row r="129">
-      <c r="E129" s="7"/>
+      <c r="F129" s="8"/>
     </row>
     <row r="130">
-      <c r="E130" s="7"/>
+      <c r="F130" s="8"/>
     </row>
     <row r="131">
-      <c r="E131" s="7"/>
+      <c r="F131" s="8"/>
     </row>
     <row r="132">
-      <c r="E132" s="7"/>
+      <c r="F132" s="8"/>
     </row>
     <row r="133">
-      <c r="E133" s="7"/>
+      <c r="F133" s="8"/>
     </row>
     <row r="134">
-      <c r="E134" s="7"/>
+      <c r="F134" s="8"/>
     </row>
     <row r="135">
-      <c r="E135" s="7"/>
+      <c r="F135" s="8"/>
     </row>
     <row r="136">
-      <c r="E136" s="7"/>
+      <c r="F136" s="8"/>
     </row>
     <row r="137">
-      <c r="E137" s="7"/>
+      <c r="F137" s="8"/>
     </row>
     <row r="138">
-      <c r="E138" s="7"/>
+      <c r="F138" s="8"/>
     </row>
     <row r="139">
-      <c r="E139" s="7"/>
+      <c r="F139" s="8"/>
     </row>
     <row r="140">
-      <c r="E140" s="7"/>
+      <c r="F140" s="8"/>
     </row>
     <row r="141">
-      <c r="E141" s="7"/>
+      <c r="F141" s="8"/>
     </row>
     <row r="142">
-      <c r="E142" s="7"/>
+      <c r="F142" s="8"/>
     </row>
     <row r="143">
-      <c r="E143" s="7"/>
+      <c r="F143" s="8"/>
     </row>
     <row r="144">
-      <c r="E144" s="7"/>
+      <c r="F144" s="8"/>
     </row>
     <row r="145">
-      <c r="E145" s="7"/>
+      <c r="F145" s="8"/>
     </row>
     <row r="146">
-      <c r="E146" s="7"/>
+      <c r="F146" s="8"/>
     </row>
     <row r="147">
-      <c r="E147" s="7"/>
+      <c r="F147" s="8"/>
     </row>
     <row r="148">
-      <c r="E148" s="7"/>
+      <c r="F148" s="8"/>
     </row>
     <row r="149">
-      <c r="E149" s="7"/>
+      <c r="F149" s="8"/>
     </row>
     <row r="150">
-      <c r="E150" s="7"/>
+      <c r="F150" s="8"/>
     </row>
     <row r="151">
-      <c r="E151" s="7"/>
+      <c r="F151" s="8"/>
     </row>
     <row r="152">
-      <c r="E152" s="7"/>
+      <c r="F152" s="8"/>
     </row>
     <row r="153">
-      <c r="E153" s="7"/>
+      <c r="F153" s="8"/>
     </row>
     <row r="154">
-      <c r="E154" s="7"/>
+      <c r="F154" s="8"/>
     </row>
     <row r="155">
-      <c r="E155" s="7"/>
+      <c r="F155" s="8"/>
     </row>
     <row r="156">
-      <c r="E156" s="7"/>
+      <c r="F156" s="8"/>
     </row>
     <row r="157">
-      <c r="E157" s="7"/>
+      <c r="F157" s="8"/>
     </row>
     <row r="158">
-      <c r="E158" s="7"/>
+      <c r="F158" s="8"/>
     </row>
     <row r="159">
-      <c r="E159" s="7"/>
+      <c r="F159" s="8"/>
     </row>
     <row r="160">
-      <c r="E160" s="7"/>
+      <c r="F160" s="8"/>
     </row>
     <row r="161">
-      <c r="E161" s="7"/>
+      <c r="F161" s="8"/>
     </row>
     <row r="162">
-      <c r="E162" s="7"/>
+      <c r="F162" s="8"/>
     </row>
     <row r="163">
-      <c r="E163" s="7"/>
+      <c r="F163" s="8"/>
     </row>
     <row r="164">
-      <c r="E164" s="7"/>
+      <c r="F164" s="8"/>
     </row>
     <row r="165">
-      <c r="E165" s="7"/>
+      <c r="F165" s="8"/>
     </row>
     <row r="166">
-      <c r="E166" s="7"/>
+      <c r="F166" s="8"/>
     </row>
     <row r="167">
-      <c r="E167" s="7"/>
+      <c r="F167" s="8"/>
     </row>
     <row r="168">
-      <c r="E168" s="7"/>
+      <c r="F168" s="8"/>
     </row>
     <row r="169">
-      <c r="E169" s="7"/>
+      <c r="F169" s="8"/>
     </row>
     <row r="170">
-      <c r="E170" s="7"/>
+      <c r="F170" s="8"/>
     </row>
     <row r="171">
-      <c r="E171" s="7"/>
+      <c r="F171" s="8"/>
     </row>
     <row r="172">
-      <c r="E172" s="7"/>
+      <c r="F172" s="8"/>
     </row>
     <row r="173">
-      <c r="E173" s="7"/>
+      <c r="F173" s="8"/>
     </row>
     <row r="174">
-      <c r="E174" s="7"/>
+      <c r="F174" s="8"/>
     </row>
     <row r="175">
-      <c r="E175" s="7"/>
+      <c r="F175" s="8"/>
     </row>
     <row r="176">
-      <c r="E176" s="7"/>
+      <c r="F176" s="8"/>
     </row>
     <row r="177">
-      <c r="E177" s="7"/>
+      <c r="F177" s="8"/>
     </row>
     <row r="178">
-      <c r="E178" s="7"/>
+      <c r="F178" s="8"/>
     </row>
     <row r="179">
-      <c r="E179" s="7"/>
+      <c r="F179" s="8"/>
     </row>
     <row r="180">
-      <c r="E180" s="7"/>
+      <c r="F180" s="8"/>
     </row>
     <row r="181">
-      <c r="E181" s="7"/>
+      <c r="F181" s="8"/>
     </row>
     <row r="182">
-      <c r="E182" s="7"/>
+      <c r="F182" s="8"/>
     </row>
     <row r="183">
-      <c r="E183" s="7"/>
+      <c r="F183" s="8"/>
     </row>
     <row r="184">
-      <c r="E184" s="7"/>
+      <c r="F184" s="8"/>
     </row>
     <row r="185">
-      <c r="E185" s="7"/>
+      <c r="F185" s="8"/>
     </row>
     <row r="186">
-      <c r="E186" s="7"/>
+      <c r="F186" s="8"/>
     </row>
     <row r="187">
-      <c r="E187" s="7"/>
+      <c r="F187" s="8"/>
     </row>
     <row r="188">
-      <c r="E188" s="7"/>
+      <c r="F188" s="8"/>
     </row>
     <row r="189">
-      <c r="E189" s="7"/>
+      <c r="F189" s="8"/>
     </row>
     <row r="190">
-      <c r="E190" s="7"/>
+      <c r="F190" s="8"/>
     </row>
     <row r="191">
-      <c r="E191" s="7"/>
+      <c r="F191" s="8"/>
     </row>
     <row r="192">
-      <c r="E192" s="7"/>
+      <c r="F192" s="8"/>
     </row>
     <row r="193">
-      <c r="E193" s="7"/>
+      <c r="F193" s="8"/>
     </row>
     <row r="194">
-      <c r="E194" s="7"/>
+      <c r="F194" s="8"/>
     </row>
     <row r="195">
-      <c r="E195" s="7"/>
+      <c r="F195" s="8"/>
     </row>
     <row r="196">
-      <c r="E196" s="7"/>
+      <c r="F196" s="8"/>
     </row>
     <row r="197">
-      <c r="E197" s="7"/>
+      <c r="F197" s="8"/>
     </row>
     <row r="198">
-      <c r="E198" s="7"/>
+      <c r="F198" s="8"/>
     </row>
     <row r="199">
-      <c r="E199" s="7"/>
+      <c r="F199" s="8"/>
     </row>
     <row r="200">
-      <c r="E200" s="7"/>
+      <c r="F200" s="8"/>
     </row>
     <row r="201">
-      <c r="E201" s="7"/>
+      <c r="F201" s="8"/>
     </row>
     <row r="202">
-      <c r="E202" s="7"/>
+      <c r="F202" s="8"/>
     </row>
     <row r="203">
-      <c r="E203" s="7"/>
+      <c r="F203" s="8"/>
     </row>
     <row r="204">
-      <c r="E204" s="7"/>
+      <c r="F204" s="8"/>
     </row>
     <row r="205">
-      <c r="E205" s="7"/>
+      <c r="F205" s="8"/>
     </row>
     <row r="206">
-      <c r="E206" s="7"/>
+      <c r="F206" s="8"/>
     </row>
     <row r="207">
-      <c r="E207" s="7"/>
+      <c r="F207" s="8"/>
     </row>
     <row r="208">
-      <c r="E208" s="7"/>
+      <c r="F208" s="8"/>
     </row>
     <row r="209">
-      <c r="E209" s="7"/>
+      <c r="F209" s="8"/>
     </row>
     <row r="210">
-      <c r="E210" s="7"/>
+      <c r="F210" s="8"/>
     </row>
     <row r="211">
-      <c r="E211" s="7"/>
+      <c r="F211" s="8"/>
     </row>
     <row r="212">
-      <c r="E212" s="7"/>
+      <c r="F212" s="8"/>
     </row>
     <row r="213">
-      <c r="E213" s="7"/>
+      <c r="F213" s="8"/>
     </row>
     <row r="214">
-      <c r="E214" s="7"/>
+      <c r="F214" s="8"/>
     </row>
     <row r="215">
-      <c r="E215" s="7"/>
+      <c r="F215" s="8"/>
     </row>
     <row r="216">
-      <c r="E216" s="7"/>
+      <c r="F216" s="8"/>
     </row>
     <row r="217">
-      <c r="E217" s="7"/>
+      <c r="F217" s="8"/>
     </row>
     <row r="218">
-      <c r="E218" s="7"/>
+      <c r="F218" s="8"/>
     </row>
     <row r="219">
-      <c r="E219" s="7"/>
+      <c r="F219" s="8"/>
     </row>
     <row r="220">
-      <c r="E220" s="7"/>
+      <c r="F220" s="8"/>
     </row>
     <row r="221">
-      <c r="E221" s="7"/>
+      <c r="F221" s="8"/>
     </row>
     <row r="222">
-      <c r="E222" s="7"/>
+      <c r="F222" s="8"/>
     </row>
     <row r="223">
-      <c r="E223" s="7"/>
+      <c r="F223" s="8"/>
     </row>
     <row r="224">
-      <c r="E224" s="7"/>
+      <c r="F224" s="8"/>
     </row>
     <row r="225">
-      <c r="E225" s="7"/>
+      <c r="F225" s="8"/>
     </row>
     <row r="226">
-      <c r="E226" s="7"/>
+      <c r="F226" s="8"/>
     </row>
     <row r="227">
-      <c r="E227" s="7"/>
+      <c r="F227" s="8"/>
     </row>
     <row r="228">
-      <c r="E228" s="7"/>
+      <c r="F228" s="8"/>
     </row>
     <row r="229">
-      <c r="E229" s="7"/>
+      <c r="F229" s="8"/>
     </row>
     <row r="230">
-      <c r="E230" s="7"/>
+      <c r="F230" s="8"/>
     </row>
     <row r="231">
-      <c r="E231" s="7"/>
+      <c r="F231" s="8"/>
     </row>
     <row r="232">
-      <c r="E232" s="7"/>
+      <c r="F232" s="8"/>
     </row>
     <row r="233">
-      <c r="E233" s="7"/>
+      <c r="F233" s="8"/>
     </row>
     <row r="234">
-      <c r="E234" s="7"/>
+      <c r="F234" s="8"/>
     </row>
     <row r="235">
-      <c r="E235" s="7"/>
+      <c r="F235" s="8"/>
     </row>
     <row r="236">
-      <c r="E236" s="7"/>
+      <c r="F236" s="8"/>
     </row>
     <row r="237">
-      <c r="E237" s="7"/>
+      <c r="F237" s="8"/>
     </row>
     <row r="238">
-      <c r="E238" s="7"/>
+      <c r="F238" s="8"/>
     </row>
     <row r="239">
-      <c r="E239" s="7"/>
+      <c r="F239" s="8"/>
     </row>
     <row r="240">
-      <c r="E240" s="7"/>
+      <c r="F240" s="8"/>
     </row>
     <row r="241">
-      <c r="E241" s="7"/>
+      <c r="F241" s="8"/>
     </row>
     <row r="242">
-      <c r="E242" s="7"/>
+      <c r="F242" s="8"/>
     </row>
     <row r="243">
-      <c r="E243" s="7"/>
+      <c r="F243" s="8"/>
     </row>
     <row r="244">
-      <c r="E244" s="7"/>
+      <c r="F244" s="8"/>
     </row>
     <row r="245">
-      <c r="E245" s="7"/>
+      <c r="F245" s="8"/>
     </row>
     <row r="246">
-      <c r="E246" s="7"/>
+      <c r="F246" s="8"/>
     </row>
     <row r="247">
-      <c r="E247" s="7"/>
+      <c r="F247" s="8"/>
     </row>
     <row r="248">
-      <c r="E248" s="7"/>
+      <c r="F248" s="8"/>
     </row>
     <row r="249">
-      <c r="E249" s="7"/>
+      <c r="F249" s="8"/>
     </row>
     <row r="250">
-      <c r="E250" s="7"/>
+      <c r="F250" s="8"/>
     </row>
     <row r="251">
-      <c r="E251" s="7"/>
+      <c r="F251" s="8"/>
     </row>
     <row r="252">
-      <c r="E252" s="7"/>
+      <c r="F252" s="8"/>
     </row>
     <row r="253">
-      <c r="E253" s="7"/>
+      <c r="F253" s="8"/>
     </row>
     <row r="254">
-      <c r="E254" s="7"/>
+      <c r="F254" s="8"/>
     </row>
     <row r="255">
-      <c r="E255" s="7"/>
+      <c r="F255" s="8"/>
     </row>
     <row r="256">
-      <c r="E256" s="7"/>
+      <c r="F256" s="8"/>
     </row>
     <row r="257">
-      <c r="E257" s="7"/>
+      <c r="F257" s="8"/>
     </row>
     <row r="258">
-      <c r="E258" s="7"/>
+      <c r="F258" s="8"/>
     </row>
     <row r="259">
-      <c r="E259" s="7"/>
+      <c r="F259" s="8"/>
     </row>
     <row r="260">
-      <c r="E260" s="7"/>
+      <c r="F260" s="8"/>
     </row>
     <row r="261">
-      <c r="E261" s="7"/>
+      <c r="F261" s="8"/>
     </row>
     <row r="262">
-      <c r="E262" s="7"/>
+      <c r="F262" s="8"/>
     </row>
     <row r="263">
-      <c r="E263" s="7"/>
+      <c r="F263" s="8"/>
     </row>
     <row r="264">
-      <c r="E264" s="7"/>
+      <c r="F264" s="8"/>
     </row>
     <row r="265">
-      <c r="E265" s="7"/>
+      <c r="F265" s="8"/>
     </row>
     <row r="266">
-      <c r="E266" s="7"/>
+      <c r="F266" s="8"/>
     </row>
     <row r="267">
-      <c r="E267" s="7"/>
+      <c r="F267" s="8"/>
     </row>
     <row r="268">
-      <c r="E268" s="7"/>
+      <c r="F268" s="8"/>
     </row>
     <row r="269">
-      <c r="E269" s="7"/>
+      <c r="F269" s="8"/>
     </row>
     <row r="270">
-      <c r="E270" s="7"/>
+      <c r="F270" s="8"/>
     </row>
     <row r="271">
-      <c r="E271" s="7"/>
+      <c r="F271" s="8"/>
     </row>
     <row r="272">
-      <c r="E272" s="7"/>
+      <c r="F272" s="8"/>
     </row>
     <row r="273">
-      <c r="E273" s="7"/>
+      <c r="F273" s="8"/>
     </row>
     <row r="274">
-      <c r="E274" s="7"/>
+      <c r="F274" s="8"/>
     </row>
     <row r="275">
-      <c r="E275" s="7"/>
+      <c r="F275" s="8"/>
     </row>
     <row r="276">
-      <c r="E276" s="7"/>
+      <c r="F276" s="8"/>
     </row>
     <row r="277">
-      <c r="E277" s="7"/>
+      <c r="F277" s="8"/>
     </row>
     <row r="278">
-      <c r="E278" s="7"/>
+      <c r="F278" s="8"/>
     </row>
     <row r="279">
-      <c r="E279" s="7"/>
+      <c r="F279" s="8"/>
     </row>
     <row r="280">
-      <c r="E280" s="7"/>
+      <c r="F280" s="8"/>
     </row>
     <row r="281">
-      <c r="E281" s="7"/>
+      <c r="F281" s="8"/>
     </row>
     <row r="282">
-      <c r="E282" s="7"/>
+      <c r="F282" s="8"/>
     </row>
     <row r="283">
-      <c r="E283" s="7"/>
+      <c r="F283" s="8"/>
     </row>
     <row r="284">
-      <c r="E284" s="7"/>
+      <c r="F284" s="8"/>
     </row>
     <row r="285">
-      <c r="E285" s="7"/>
+      <c r="F285" s="8"/>
     </row>
     <row r="286">
-      <c r="E286" s="7"/>
+      <c r="F286" s="8"/>
     </row>
     <row r="287">
-      <c r="E287" s="7"/>
+      <c r="F287" s="8"/>
     </row>
     <row r="288">
-      <c r="E288" s="7"/>
+      <c r="F288" s="8"/>
     </row>
     <row r="289">
-      <c r="E289" s="7"/>
+      <c r="F289" s="8"/>
     </row>
     <row r="290">
-      <c r="E290" s="7"/>
+      <c r="F290" s="8"/>
     </row>
     <row r="291">
-      <c r="E291" s="7"/>
+      <c r="F291" s="8"/>
     </row>
     <row r="292">
-      <c r="E292" s="7"/>
+      <c r="F292" s="8"/>
     </row>
     <row r="293">
-      <c r="E293" s="7"/>
+      <c r="F293" s="8"/>
     </row>
     <row r="294">
-      <c r="E294" s="7"/>
+      <c r="F294" s="8"/>
     </row>
     <row r="295">
-      <c r="E295" s="7"/>
+      <c r="F295" s="8"/>
     </row>
     <row r="296">
-      <c r="E296" s="7"/>
+      <c r="F296" s="8"/>
     </row>
     <row r="297">
-      <c r="E297" s="7"/>
+      <c r="F297" s="8"/>
     </row>
     <row r="298">
-      <c r="E298" s="7"/>
+      <c r="F298" s="8"/>
     </row>
     <row r="299">
-      <c r="E299" s="7"/>
+      <c r="F299" s="8"/>
     </row>
     <row r="300">
-      <c r="E300" s="7"/>
+      <c r="F300" s="8"/>
     </row>
     <row r="301">
-      <c r="E301" s="7"/>
+      <c r="F301" s="8"/>
     </row>
     <row r="302">
-      <c r="E302" s="7"/>
+      <c r="F302" s="8"/>
     </row>
     <row r="303">
-      <c r="E303" s="7"/>
+      <c r="F303" s="8"/>
     </row>
     <row r="304">
-      <c r="E304" s="7"/>
+      <c r="F304" s="8"/>
     </row>
     <row r="305">
-      <c r="E305" s="7"/>
+      <c r="F305" s="8"/>
     </row>
     <row r="306">
-      <c r="E306" s="7"/>
+      <c r="F306" s="8"/>
     </row>
     <row r="307">
-      <c r="E307" s="7"/>
+      <c r="F307" s="8"/>
     </row>
     <row r="308">
-      <c r="E308" s="7"/>
+      <c r="F308" s="8"/>
     </row>
     <row r="309">
-      <c r="E309" s="7"/>
+      <c r="F309" s="8"/>
     </row>
     <row r="310">
-      <c r="E310" s="7"/>
+      <c r="F310" s="8"/>
     </row>
     <row r="311">
-      <c r="E311" s="7"/>
+      <c r="F311" s="8"/>
     </row>
     <row r="312">
-      <c r="E312" s="7"/>
+      <c r="F312" s="8"/>
     </row>
     <row r="313">
-      <c r="E313" s="7"/>
+      <c r="F313" s="8"/>
     </row>
     <row r="314">
-      <c r="E314" s="7"/>
+      <c r="F314" s="8"/>
     </row>
     <row r="315">
-      <c r="E315" s="7"/>
+      <c r="F315" s="8"/>
     </row>
     <row r="316">
-      <c r="E316" s="7"/>
+      <c r="F316" s="8"/>
     </row>
     <row r="317">
-      <c r="E317" s="7"/>
+      <c r="F317" s="8"/>
     </row>
     <row r="318">
-      <c r="E318" s="7"/>
+      <c r="F318" s="8"/>
     </row>
     <row r="319">
-      <c r="E319" s="7"/>
+      <c r="F319" s="8"/>
     </row>
     <row r="320">
-      <c r="E320" s="7"/>
+      <c r="F320" s="8"/>
     </row>
     <row r="321">
-      <c r="E321" s="7"/>
+      <c r="F321" s="8"/>
     </row>
     <row r="322">
-      <c r="E322" s="7"/>
+      <c r="F322" s="8"/>
     </row>
     <row r="323">
-      <c r="E323" s="7"/>
+      <c r="F323" s="8"/>
     </row>
     <row r="324">
-      <c r="E324" s="7"/>
+      <c r="F324" s="8"/>
     </row>
     <row r="325">
-      <c r="E325" s="7"/>
+      <c r="F325" s="8"/>
     </row>
     <row r="326">
-      <c r="E326" s="7"/>
+      <c r="F326" s="8"/>
     </row>
     <row r="327">
-      <c r="E327" s="7"/>
+      <c r="F327" s="8"/>
     </row>
     <row r="328">
-      <c r="E328" s="7"/>
+      <c r="F328" s="8"/>
     </row>
     <row r="329">
-      <c r="E329" s="7"/>
+      <c r="F329" s="8"/>
     </row>
     <row r="330">
-      <c r="E330" s="7"/>
+      <c r="F330" s="8"/>
     </row>
     <row r="331">
-      <c r="E331" s="7"/>
+      <c r="F331" s="8"/>
     </row>
     <row r="332">
-      <c r="E332" s="7"/>
+      <c r="F332" s="8"/>
     </row>
     <row r="333">
-      <c r="E333" s="7"/>
+      <c r="F333" s="8"/>
     </row>
     <row r="334">
-      <c r="E334" s="7"/>
+      <c r="F334" s="8"/>
     </row>
     <row r="335">
-      <c r="E335" s="7"/>
+      <c r="F335" s="8"/>
     </row>
     <row r="336">
-      <c r="E336" s="7"/>
+      <c r="F336" s="8"/>
     </row>
     <row r="337">
-      <c r="E337" s="7"/>
+      <c r="F337" s="8"/>
     </row>
     <row r="338">
-      <c r="E338" s="7"/>
+      <c r="F338" s="8"/>
     </row>
     <row r="339">
-      <c r="E339" s="7"/>
+      <c r="F339" s="8"/>
     </row>
     <row r="340">
-      <c r="E340" s="7"/>
+      <c r="F340" s="8"/>
     </row>
     <row r="341">
-      <c r="E341" s="7"/>
+      <c r="F341" s="8"/>
     </row>
     <row r="342">
-      <c r="E342" s="7"/>
+      <c r="F342" s="8"/>
     </row>
     <row r="343">
-      <c r="E343" s="7"/>
+      <c r="F343" s="8"/>
     </row>
     <row r="344">
-      <c r="E344" s="7"/>
+      <c r="F344" s="8"/>
     </row>
     <row r="345">
-      <c r="E345" s="7"/>
+      <c r="F345" s="8"/>
     </row>
     <row r="346">
-      <c r="E346" s="7"/>
+      <c r="F346" s="8"/>
     </row>
     <row r="347">
-      <c r="E347" s="7"/>
+      <c r="F347" s="8"/>
     </row>
     <row r="348">
-      <c r="E348" s="7"/>
+      <c r="F348" s="8"/>
     </row>
     <row r="349">
-      <c r="E349" s="7"/>
+      <c r="F349" s="8"/>
     </row>
     <row r="350">
-      <c r="E350" s="7"/>
+      <c r="F350" s="8"/>
     </row>
     <row r="351">
-      <c r="E351" s="7"/>
+      <c r="F351" s="8"/>
     </row>
     <row r="352">
-      <c r="E352" s="7"/>
+      <c r="F352" s="8"/>
     </row>
     <row r="353">
-      <c r="E353" s="7"/>
+      <c r="F353" s="8"/>
     </row>
     <row r="354">
-      <c r="E354" s="7"/>
+      <c r="F354" s="8"/>
     </row>
     <row r="355">
-      <c r="E355" s="7"/>
+      <c r="F355" s="8"/>
     </row>
     <row r="356">
-      <c r="E356" s="7"/>
+      <c r="F356" s="8"/>
     </row>
     <row r="357">
-      <c r="E357" s="7"/>
+      <c r="F357" s="8"/>
     </row>
     <row r="358">
-      <c r="E358" s="7"/>
+      <c r="F358" s="8"/>
     </row>
     <row r="359">
-      <c r="E359" s="7"/>
+      <c r="F359" s="8"/>
     </row>
     <row r="360">
-      <c r="E360" s="7"/>
+      <c r="F360" s="8"/>
     </row>
     <row r="361">
-      <c r="E361" s="7"/>
+      <c r="F361" s="8"/>
     </row>
     <row r="362">
-      <c r="E362" s="7"/>
+      <c r="F362" s="8"/>
     </row>
     <row r="363">
-      <c r="E363" s="7"/>
+      <c r="F363" s="8"/>
     </row>
     <row r="364">
-      <c r="E364" s="7"/>
+      <c r="F364" s="8"/>
     </row>
     <row r="365">
-      <c r="E365" s="7"/>
+      <c r="F365" s="8"/>
     </row>
     <row r="366">
-      <c r="E366" s="7"/>
+      <c r="F366" s="8"/>
     </row>
     <row r="367">
-      <c r="E367" s="7"/>
+      <c r="F367" s="8"/>
     </row>
     <row r="368">
-      <c r="E368" s="7"/>
+      <c r="F368" s="8"/>
     </row>
     <row r="369">
-      <c r="E369" s="7"/>
+      <c r="F369" s="8"/>
     </row>
     <row r="370">
-      <c r="E370" s="7"/>
+      <c r="F370" s="8"/>
     </row>
     <row r="371">
-      <c r="E371" s="7"/>
+      <c r="F371" s="8"/>
     </row>
     <row r="372">
-      <c r="E372" s="7"/>
+      <c r="F372" s="8"/>
     </row>
     <row r="373">
-      <c r="E373" s="7"/>
+      <c r="F373" s="8"/>
     </row>
     <row r="374">
-      <c r="E374" s="7"/>
+      <c r="F374" s="8"/>
     </row>
     <row r="375">
-      <c r="E375" s="7"/>
+      <c r="F375" s="8"/>
     </row>
     <row r="376">
-      <c r="E376" s="7"/>
+      <c r="F376" s="8"/>
     </row>
     <row r="377">
-      <c r="E377" s="7"/>
+      <c r="F377" s="8"/>
     </row>
     <row r="378">
-      <c r="E378" s="7"/>
+      <c r="F378" s="8"/>
     </row>
     <row r="379">
-      <c r="E379" s="7"/>
+      <c r="F379" s="8"/>
     </row>
     <row r="380">
-      <c r="E380" s="7"/>
+      <c r="F380" s="8"/>
     </row>
     <row r="381">
-      <c r="E381" s="7"/>
+      <c r="F381" s="8"/>
     </row>
     <row r="382">
-      <c r="E382" s="7"/>
+      <c r="F382" s="8"/>
     </row>
     <row r="383">
-      <c r="E383" s="7"/>
+      <c r="F383" s="8"/>
     </row>
     <row r="384">
-      <c r="E384" s="7"/>
+      <c r="F384" s="8"/>
     </row>
     <row r="385">
-      <c r="E385" s="7"/>
+      <c r="F385" s="8"/>
     </row>
     <row r="386">
-      <c r="E386" s="7"/>
+      <c r="F386" s="8"/>
     </row>
     <row r="387">
-      <c r="E387" s="7"/>
+      <c r="F387" s="8"/>
     </row>
     <row r="388">
-      <c r="E388" s="7"/>
+      <c r="F388" s="8"/>
     </row>
     <row r="389">
-      <c r="E389" s="7"/>
+      <c r="F389" s="8"/>
     </row>
     <row r="390">
-      <c r="E390" s="7"/>
+      <c r="F390" s="8"/>
     </row>
     <row r="391">
-      <c r="E391" s="7"/>
+      <c r="F391" s="8"/>
     </row>
     <row r="392">
-      <c r="E392" s="7"/>
+      <c r="F392" s="8"/>
     </row>
     <row r="393">
-      <c r="E393" s="7"/>
+      <c r="F393" s="8"/>
     </row>
     <row r="394">
-      <c r="E394" s="7"/>
+      <c r="F394" s="8"/>
     </row>
     <row r="395">
-      <c r="E395" s="7"/>
+      <c r="F395" s="8"/>
     </row>
     <row r="396">
-      <c r="E396" s="7"/>
+      <c r="F396" s="8"/>
     </row>
     <row r="397">
-      <c r="E397" s="7"/>
+      <c r="F397" s="8"/>
     </row>
     <row r="398">
-      <c r="E398" s="7"/>
+      <c r="F398" s="8"/>
     </row>
     <row r="399">
-      <c r="E399" s="7"/>
+      <c r="F399" s="8"/>
     </row>
     <row r="400">
-      <c r="E400" s="7"/>
+      <c r="F400" s="8"/>
     </row>
     <row r="401">
-      <c r="E401" s="7"/>
+      <c r="F401" s="8"/>
     </row>
     <row r="402">
-      <c r="E402" s="7"/>
+      <c r="F402" s="8"/>
     </row>
     <row r="403">
-      <c r="E403" s="7"/>
+      <c r="F403" s="8"/>
     </row>
     <row r="404">
-      <c r="E404" s="7"/>
+      <c r="F404" s="8"/>
     </row>
     <row r="405">
-      <c r="E405" s="7"/>
+      <c r="F405" s="8"/>
     </row>
     <row r="406">
-      <c r="E406" s="7"/>
+      <c r="F406" s="8"/>
     </row>
     <row r="407">
-      <c r="E407" s="7"/>
+      <c r="F407" s="8"/>
     </row>
     <row r="408">
-      <c r="E408" s="7"/>
+      <c r="F408" s="8"/>
     </row>
     <row r="409">
-      <c r="E409" s="7"/>
+      <c r="F409" s="8"/>
     </row>
     <row r="410">
-      <c r="E410" s="7"/>
+      <c r="F410" s="8"/>
     </row>
     <row r="411">
-      <c r="E411" s="7"/>
+      <c r="F411" s="8"/>
     </row>
     <row r="412">
-      <c r="E412" s="7"/>
+      <c r="F412" s="8"/>
     </row>
     <row r="413">
-      <c r="E413" s="7"/>
+      <c r="F413" s="8"/>
     </row>
     <row r="414">
-      <c r="E414" s="7"/>
+      <c r="F414" s="8"/>
     </row>
     <row r="415">
-      <c r="E415" s="7"/>
+      <c r="F415" s="8"/>
     </row>
     <row r="416">
-      <c r="E416" s="7"/>
+      <c r="F416" s="8"/>
     </row>
     <row r="417">
-      <c r="E417" s="7"/>
+      <c r="F417" s="8"/>
     </row>
     <row r="418">
-      <c r="E418" s="7"/>
+      <c r="F418" s="8"/>
     </row>
     <row r="419">
-      <c r="E419" s="7"/>
+      <c r="F419" s="8"/>
     </row>
     <row r="420">
-      <c r="E420" s="7"/>
+      <c r="F420" s="8"/>
     </row>
     <row r="421">
-      <c r="E421" s="7"/>
+      <c r="F421" s="8"/>
     </row>
     <row r="422">
-      <c r="E422" s="7"/>
+      <c r="F422" s="8"/>
     </row>
     <row r="423">
-      <c r="E423" s="7"/>
+      <c r="F423" s="8"/>
     </row>
     <row r="424">
-      <c r="E424" s="7"/>
+      <c r="F424" s="8"/>
     </row>
     <row r="425">
-      <c r="E425" s="7"/>
+      <c r="F425" s="8"/>
     </row>
     <row r="426">
-      <c r="E426" s="7"/>
+      <c r="F426" s="8"/>
     </row>
     <row r="427">
-      <c r="E427" s="7"/>
+      <c r="F427" s="8"/>
     </row>
     <row r="428">
-      <c r="E428" s="7"/>
+      <c r="F428" s="8"/>
     </row>
     <row r="429">
-      <c r="E429" s="7"/>
+      <c r="F429" s="8"/>
     </row>
     <row r="430">
-      <c r="E430" s="7"/>
+      <c r="F430" s="8"/>
     </row>
     <row r="431">
-      <c r="E431" s="7"/>
+      <c r="F431" s="8"/>
     </row>
     <row r="432">
-      <c r="E432" s="7"/>
+      <c r="F432" s="8"/>
     </row>
     <row r="433">
-      <c r="E433" s="7"/>
+      <c r="F433" s="8"/>
     </row>
     <row r="434">
-      <c r="E434" s="7"/>
+      <c r="F434" s="8"/>
     </row>
     <row r="435">
-      <c r="E435" s="7"/>
+      <c r="F435" s="8"/>
     </row>
     <row r="436">
-      <c r="E436" s="7"/>
+      <c r="F436" s="8"/>
     </row>
     <row r="437">
-      <c r="E437" s="7"/>
+      <c r="F437" s="8"/>
     </row>
     <row r="438">
-      <c r="E438" s="7"/>
+      <c r="F438" s="8"/>
     </row>
     <row r="439">
-      <c r="E439" s="7"/>
+      <c r="F439" s="8"/>
     </row>
     <row r="440">
-      <c r="E440" s="7"/>
+      <c r="F440" s="8"/>
     </row>
     <row r="441">
-      <c r="E441" s="7"/>
+      <c r="F441" s="8"/>
     </row>
     <row r="442">
-      <c r="E442" s="7"/>
+      <c r="F442" s="8"/>
     </row>
     <row r="443">
-      <c r="E443" s="7"/>
+      <c r="F443" s="8"/>
     </row>
     <row r="444">
-      <c r="E444" s="7"/>
+      <c r="F444" s="8"/>
     </row>
     <row r="445">
-      <c r="E445" s="7"/>
+      <c r="F445" s="8"/>
     </row>
     <row r="446">
-      <c r="E446" s="7"/>
+      <c r="F446" s="8"/>
     </row>
     <row r="447">
-      <c r="E447" s="7"/>
+      <c r="F447" s="8"/>
     </row>
     <row r="448">
-      <c r="E448" s="7"/>
+      <c r="F448" s="8"/>
     </row>
     <row r="449">
-      <c r="E449" s="7"/>
+      <c r="F449" s="8"/>
     </row>
     <row r="450">
-      <c r="E450" s="7"/>
+      <c r="F450" s="8"/>
     </row>
     <row r="451">
-      <c r="E451" s="7"/>
+      <c r="F451" s="8"/>
     </row>
     <row r="452">
-      <c r="E452" s="7"/>
+      <c r="F452" s="8"/>
     </row>
     <row r="453">
-      <c r="E453" s="7"/>
+      <c r="F453" s="8"/>
     </row>
     <row r="454">
-      <c r="E454" s="7"/>
+      <c r="F454" s="8"/>
     </row>
     <row r="455">
-      <c r="E455" s="7"/>
+      <c r="F455" s="8"/>
     </row>
     <row r="456">
-      <c r="E456" s="7"/>
+      <c r="F456" s="8"/>
     </row>
     <row r="457">
-      <c r="E457" s="7"/>
+      <c r="F457" s="8"/>
     </row>
     <row r="458">
-      <c r="E458" s="7"/>
+      <c r="F458" s="8"/>
     </row>
     <row r="459">
-      <c r="E459" s="7"/>
+      <c r="F459" s="8"/>
     </row>
     <row r="460">
-      <c r="E460" s="7"/>
+      <c r="F460" s="8"/>
     </row>
     <row r="461">
-      <c r="E461" s="7"/>
+      <c r="F461" s="8"/>
     </row>
     <row r="462">
-      <c r="E462" s="7"/>
+      <c r="F462" s="8"/>
     </row>
     <row r="463">
-      <c r="E463" s="7"/>
+      <c r="F463" s="8"/>
     </row>
     <row r="464">
-      <c r="E464" s="7"/>
+      <c r="F464" s="8"/>
     </row>
     <row r="465">
-      <c r="E465" s="7"/>
+      <c r="F465" s="8"/>
     </row>
     <row r="466">
-      <c r="E466" s="7"/>
+      <c r="F466" s="8"/>
     </row>
     <row r="467">
-      <c r="E467" s="7"/>
+      <c r="F467" s="8"/>
     </row>
     <row r="468">
-      <c r="E468" s="7"/>
+      <c r="F468" s="8"/>
     </row>
     <row r="469">
-      <c r="E469" s="7"/>
+      <c r="F469" s="8"/>
     </row>
     <row r="470">
-      <c r="E470" s="7"/>
+      <c r="F470" s="8"/>
     </row>
     <row r="471">
-      <c r="E471" s="7"/>
+      <c r="F471" s="8"/>
     </row>
     <row r="472">
-      <c r="E472" s="7"/>
+      <c r="F472" s="8"/>
     </row>
     <row r="473">
-      <c r="E473" s="7"/>
+      <c r="F473" s="8"/>
     </row>
     <row r="474">
-      <c r="E474" s="7"/>
+      <c r="F474" s="8"/>
     </row>
     <row r="475">
-      <c r="E475" s="7"/>
+      <c r="F475" s="8"/>
     </row>
     <row r="476">
-      <c r="E476" s="7"/>
+      <c r="F476" s="8"/>
     </row>
     <row r="477">
-      <c r="E477" s="7"/>
+      <c r="F477" s="8"/>
     </row>
     <row r="478">
-      <c r="E478" s="7"/>
+      <c r="F478" s="8"/>
     </row>
     <row r="479">
-      <c r="E479" s="7"/>
+      <c r="F479" s="8"/>
     </row>
     <row r="480">
-      <c r="E480" s="7"/>
+      <c r="F480" s="8"/>
     </row>
     <row r="481">
-      <c r="E481" s="7"/>
+      <c r="F481" s="8"/>
     </row>
     <row r="482">
-      <c r="E482" s="7"/>
+      <c r="F482" s="8"/>
     </row>
     <row r="483">
-      <c r="E483" s="7"/>
+      <c r="F483" s="8"/>
     </row>
     <row r="484">
-      <c r="E484" s="7"/>
+      <c r="F484" s="8"/>
     </row>
     <row r="485">
-      <c r="E485" s="7"/>
+      <c r="F485" s="8"/>
     </row>
     <row r="486">
-      <c r="E486" s="7"/>
+      <c r="F486" s="8"/>
     </row>
     <row r="487">
-      <c r="E487" s="7"/>
+      <c r="F487" s="8"/>
     </row>
     <row r="488">
-      <c r="E488" s="7"/>
+      <c r="F488" s="8"/>
     </row>
     <row r="489">
-      <c r="E489" s="7"/>
+      <c r="F489" s="8"/>
     </row>
     <row r="490">
-      <c r="E490" s="7"/>
+      <c r="F490" s="8"/>
     </row>
     <row r="491">
-      <c r="E491" s="7"/>
+      <c r="F491" s="8"/>
     </row>
     <row r="492">
-      <c r="E492" s="7"/>
+      <c r="F492" s="8"/>
     </row>
     <row r="493">
-      <c r="E493" s="7"/>
+      <c r="F493" s="8"/>
     </row>
     <row r="494">
-      <c r="E494" s="7"/>
+      <c r="F494" s="8"/>
     </row>
     <row r="495">
-      <c r="E495" s="7"/>
+      <c r="F495" s="8"/>
     </row>
     <row r="496">
-      <c r="E496" s="7"/>
+      <c r="F496" s="8"/>
     </row>
     <row r="497">
-      <c r="E497" s="7"/>
+      <c r="F497" s="8"/>
     </row>
     <row r="498">
-      <c r="E498" s="7"/>
+      <c r="F498" s="8"/>
     </row>
     <row r="499">
-      <c r="E499" s="7"/>
+      <c r="F499" s="8"/>
     </row>
     <row r="500">
-      <c r="E500" s="7"/>
+      <c r="F500" s="8"/>
     </row>
     <row r="501">
-      <c r="E501" s="7"/>
+      <c r="F501" s="8"/>
     </row>
     <row r="502">
-      <c r="E502" s="7"/>
+      <c r="F502" s="8"/>
     </row>
     <row r="503">
-      <c r="E503" s="7"/>
+      <c r="F503" s="8"/>
     </row>
     <row r="504">
-      <c r="E504" s="7"/>
+      <c r="F504" s="8"/>
     </row>
     <row r="505">
-      <c r="E505" s="7"/>
+      <c r="F505" s="8"/>
     </row>
     <row r="506">
-      <c r="E506" s="7"/>
+      <c r="F506" s="8"/>
     </row>
     <row r="507">
-      <c r="E507" s="7"/>
+      <c r="F507" s="8"/>
     </row>
     <row r="508">
-      <c r="E508" s="7"/>
+      <c r="F508" s="8"/>
     </row>
     <row r="509">
-      <c r="E509" s="7"/>
+      <c r="F509" s="8"/>
     </row>
     <row r="510">
-      <c r="E510" s="7"/>
+      <c r="F510" s="8"/>
     </row>
     <row r="511">
-      <c r="E511" s="7"/>
+      <c r="F511" s="8"/>
     </row>
     <row r="512">
-      <c r="E512" s="7"/>
+      <c r="F512" s="8"/>
     </row>
     <row r="513">
-      <c r="E513" s="7"/>
+      <c r="F513" s="8"/>
     </row>
     <row r="514">
-      <c r="E514" s="7"/>
+      <c r="F514" s="8"/>
     </row>
     <row r="515">
-      <c r="E515" s="7"/>
+      <c r="F515" s="8"/>
     </row>
     <row r="516">
-      <c r="E516" s="7"/>
+      <c r="F516" s="8"/>
     </row>
     <row r="517">
-      <c r="E517" s="7"/>
+      <c r="F517" s="8"/>
     </row>
     <row r="518">
-      <c r="E518" s="7"/>
+      <c r="F518" s="8"/>
     </row>
     <row r="519">
-      <c r="E519" s="7"/>
+      <c r="F519" s="8"/>
     </row>
     <row r="520">
-      <c r="E520" s="7"/>
+      <c r="F520" s="8"/>
     </row>
     <row r="521">
-      <c r="E521" s="7"/>
+      <c r="F521" s="8"/>
     </row>
     <row r="522">
-      <c r="E522" s="7"/>
+      <c r="F522" s="8"/>
     </row>
     <row r="523">
-      <c r="E523" s="7"/>
+      <c r="F523" s="8"/>
     </row>
     <row r="524">
-      <c r="E524" s="7"/>
+      <c r="F524" s="8"/>
     </row>
     <row r="525">
-      <c r="E525" s="7"/>
+      <c r="F525" s="8"/>
     </row>
     <row r="526">
-      <c r="E526" s="7"/>
+      <c r="F526" s="8"/>
     </row>
     <row r="527">
-      <c r="E527" s="7"/>
+      <c r="F527" s="8"/>
     </row>
     <row r="528">
-      <c r="E528" s="7"/>
+      <c r="F528" s="8"/>
     </row>
     <row r="529">
-      <c r="E529" s="7"/>
+      <c r="F529" s="8"/>
     </row>
     <row r="530">
-      <c r="E530" s="7"/>
+      <c r="F530" s="8"/>
     </row>
     <row r="531">
-      <c r="E531" s="7"/>
+      <c r="F531" s="8"/>
     </row>
     <row r="532">
-      <c r="E532" s="7"/>
+      <c r="F532" s="8"/>
     </row>
     <row r="533">
-      <c r="E533" s="7"/>
+      <c r="F533" s="8"/>
     </row>
     <row r="534">
-      <c r="E534" s="7"/>
+      <c r="F534" s="8"/>
     </row>
     <row r="535">
-      <c r="E535" s="7"/>
+      <c r="F535" s="8"/>
     </row>
     <row r="536">
-      <c r="E536" s="7"/>
+      <c r="F536" s="8"/>
     </row>
     <row r="537">
-      <c r="E537" s="7"/>
+      <c r="F537" s="8"/>
     </row>
     <row r="538">
-      <c r="E538" s="7"/>
+      <c r="F538" s="8"/>
     </row>
     <row r="539">
-      <c r="E539" s="7"/>
+      <c r="F539" s="8"/>
     </row>
     <row r="540">
-      <c r="E540" s="7"/>
+      <c r="F540" s="8"/>
     </row>
     <row r="541">
-      <c r="E541" s="7"/>
+      <c r="F541" s="8"/>
     </row>
     <row r="542">
-      <c r="E542" s="7"/>
+      <c r="F542" s="8"/>
     </row>
     <row r="543">
-      <c r="E543" s="7"/>
+      <c r="F543" s="8"/>
     </row>
     <row r="544">
-      <c r="E544" s="7"/>
+      <c r="F544" s="8"/>
     </row>
     <row r="545">
-      <c r="E545" s="7"/>
+      <c r="F545" s="8"/>
     </row>
     <row r="546">
-      <c r="E546" s="7"/>
+      <c r="F546" s="8"/>
     </row>
     <row r="547">
-      <c r="E547" s="7"/>
+      <c r="F547" s="8"/>
     </row>
     <row r="548">
-      <c r="E548" s="7"/>
+      <c r="F548" s="8"/>
     </row>
     <row r="549">
-      <c r="E549" s="7"/>
+      <c r="F549" s="8"/>
     </row>
     <row r="550">
-      <c r="E550" s="7"/>
+      <c r="F550" s="8"/>
     </row>
     <row r="551">
-      <c r="E551" s="7"/>
+      <c r="F551" s="8"/>
     </row>
     <row r="552">
-      <c r="E552" s="7"/>
+      <c r="F552" s="8"/>
     </row>
     <row r="553">
-      <c r="E553" s="7"/>
+      <c r="F553" s="8"/>
     </row>
     <row r="554">
-      <c r="E554" s="7"/>
+      <c r="F554" s="8"/>
     </row>
     <row r="555">
-      <c r="E555" s="7"/>
+      <c r="F555" s="8"/>
     </row>
     <row r="556">
-      <c r="E556" s="7"/>
+      <c r="F556" s="8"/>
     </row>
     <row r="557">
-      <c r="E557" s="7"/>
+      <c r="F557" s="8"/>
     </row>
     <row r="558">
-      <c r="E558" s="7"/>
+      <c r="F558" s="8"/>
     </row>
     <row r="559">
-      <c r="E559" s="7"/>
+      <c r="F559" s="8"/>
     </row>
     <row r="560">
-      <c r="E560" s="7"/>
+      <c r="F560" s="8"/>
     </row>
     <row r="561">
-      <c r="E561" s="7"/>
+      <c r="F561" s="8"/>
     </row>
     <row r="562">
-      <c r="E562" s="7"/>
+      <c r="F562" s="8"/>
     </row>
     <row r="563">
-      <c r="E563" s="7"/>
+      <c r="F563" s="8"/>
     </row>
     <row r="564">
-      <c r="E564" s="7"/>
+      <c r="F564" s="8"/>
     </row>
     <row r="565">
-      <c r="E565" s="7"/>
+      <c r="F565" s="8"/>
     </row>
     <row r="566">
-      <c r="E566" s="7"/>
+      <c r="F566" s="8"/>
     </row>
     <row r="567">
-      <c r="E567" s="7"/>
+      <c r="F567" s="8"/>
     </row>
     <row r="568">
-      <c r="E568" s="7"/>
+      <c r="F568" s="8"/>
     </row>
     <row r="569">
-      <c r="E569" s="7"/>
+      <c r="F569" s="8"/>
     </row>
     <row r="570">
-      <c r="E570" s="7"/>
+      <c r="F570" s="8"/>
     </row>
     <row r="571">
-      <c r="E571" s="7"/>
+      <c r="F571" s="8"/>
     </row>
     <row r="572">
-      <c r="E572" s="7"/>
+      <c r="F572" s="8"/>
     </row>
     <row r="573">
-      <c r="E573" s="7"/>
+      <c r="F573" s="8"/>
     </row>
     <row r="574">
-      <c r="E574" s="7"/>
+      <c r="F574" s="8"/>
     </row>
     <row r="575">
-      <c r="E575" s="7"/>
+      <c r="F575" s="8"/>
     </row>
     <row r="576">
-      <c r="E576" s="7"/>
+      <c r="F576" s="8"/>
     </row>
     <row r="577">
-      <c r="E577" s="7"/>
+      <c r="F577" s="8"/>
     </row>
     <row r="578">
-      <c r="E578" s="7"/>
+      <c r="F578" s="8"/>
     </row>
     <row r="579">
-      <c r="E579" s="7"/>
+      <c r="F579" s="8"/>
     </row>
     <row r="580">
-      <c r="E580" s="7"/>
+      <c r="F580" s="8"/>
     </row>
     <row r="581">
-      <c r="E581" s="7"/>
+      <c r="F581" s="8"/>
     </row>
     <row r="582">
-      <c r="E582" s="7"/>
+      <c r="F582" s="8"/>
     </row>
     <row r="583">
-      <c r="E583" s="7"/>
+      <c r="F583" s="8"/>
     </row>
     <row r="584">
-      <c r="E584" s="7"/>
+      <c r="F584" s="8"/>
     </row>
     <row r="585">
-      <c r="E585" s="7"/>
+      <c r="F585" s="8"/>
     </row>
     <row r="586">
-      <c r="E586" s="7"/>
+      <c r="F586" s="8"/>
     </row>
     <row r="587">
-      <c r="E587" s="7"/>
+      <c r="F587" s="8"/>
     </row>
     <row r="588">
-      <c r="E588" s="7"/>
+      <c r="F588" s="8"/>
     </row>
     <row r="589">
-      <c r="E589" s="7"/>
+      <c r="F589" s="8"/>
     </row>
     <row r="590">
-      <c r="E590" s="7"/>
+      <c r="F590" s="8"/>
     </row>
     <row r="591">
-      <c r="E591" s="7"/>
+      <c r="F591" s="8"/>
     </row>
     <row r="592">
-      <c r="E592" s="7"/>
+      <c r="F592" s="8"/>
     </row>
     <row r="593">
-      <c r="E593" s="7"/>
+      <c r="F593" s="8"/>
     </row>
     <row r="594">
-      <c r="E594" s="7"/>
+      <c r="F594" s="8"/>
     </row>
     <row r="595">
-      <c r="E595" s="7"/>
+      <c r="F595" s="8"/>
     </row>
     <row r="596">
-      <c r="E596" s="7"/>
+      <c r="F596" s="8"/>
     </row>
     <row r="597">
-      <c r="E597" s="7"/>
+      <c r="F597" s="8"/>
     </row>
     <row r="598">
-      <c r="E598" s="7"/>
+      <c r="F598" s="8"/>
     </row>
     <row r="599">
-      <c r="E599" s="7"/>
+      <c r="F599" s="8"/>
     </row>
     <row r="600">
-      <c r="E600" s="7"/>
+      <c r="F600" s="8"/>
     </row>
     <row r="601">
-      <c r="E601" s="7"/>
+      <c r="F601" s="8"/>
     </row>
     <row r="602">
-      <c r="E602" s="7"/>
+      <c r="F602" s="8"/>
     </row>
     <row r="603">
-      <c r="E603" s="7"/>
+      <c r="F603" s="8"/>
     </row>
     <row r="604">
-      <c r="E604" s="7"/>
+      <c r="F604" s="8"/>
     </row>
     <row r="605">
-      <c r="E605" s="7"/>
+      <c r="F605" s="8"/>
     </row>
     <row r="606">
-      <c r="E606" s="7"/>
+      <c r="F606" s="8"/>
     </row>
     <row r="607">
-      <c r="E607" s="7"/>
+      <c r="F607" s="8"/>
     </row>
     <row r="608">
-      <c r="E608" s="7"/>
+      <c r="F608" s="8"/>
     </row>
     <row r="609">
-      <c r="E609" s="7"/>
+      <c r="F609" s="8"/>
     </row>
     <row r="610">
-      <c r="E610" s="7"/>
+      <c r="F610" s="8"/>
     </row>
     <row r="611">
-      <c r="E611" s="7"/>
+      <c r="F611" s="8"/>
     </row>
     <row r="612">
-      <c r="E612" s="7"/>
+      <c r="F612" s="8"/>
     </row>
     <row r="613">
-      <c r="E613" s="7"/>
+      <c r="F613" s="8"/>
     </row>
     <row r="614">
-      <c r="E614" s="7"/>
+      <c r="F614" s="8"/>
     </row>
     <row r="615">
-      <c r="E615" s="7"/>
+      <c r="F615" s="8"/>
     </row>
     <row r="616">
-      <c r="E616" s="7"/>
+      <c r="F616" s="8"/>
     </row>
     <row r="617">
-      <c r="E617" s="7"/>
+      <c r="F617" s="8"/>
     </row>
     <row r="618">
-      <c r="E618" s="7"/>
+      <c r="F618" s="8"/>
     </row>
     <row r="619">
-      <c r="E619" s="7"/>
+      <c r="F619" s="8"/>
     </row>
     <row r="620">
-      <c r="E620" s="7"/>
+      <c r="F620" s="8"/>
     </row>
     <row r="621">
-      <c r="E621" s="7"/>
+      <c r="F621" s="8"/>
     </row>
     <row r="622">
-      <c r="E622" s="7"/>
+      <c r="F622" s="8"/>
     </row>
     <row r="623">
-      <c r="E623" s="7"/>
+      <c r="F623" s="8"/>
     </row>
     <row r="624">
-      <c r="E624" s="7"/>
+      <c r="F624" s="8"/>
     </row>
     <row r="625">
-      <c r="E625" s="7"/>
+      <c r="F625" s="8"/>
     </row>
     <row r="626">
-      <c r="E626" s="7"/>
+      <c r="F626" s="8"/>
     </row>
     <row r="627">
-      <c r="E627" s="7"/>
+      <c r="F627" s="8"/>
     </row>
     <row r="628">
-      <c r="E628" s="7"/>
+      <c r="F628" s="8"/>
     </row>
     <row r="629">
-      <c r="E629" s="7"/>
+      <c r="F629" s="8"/>
     </row>
     <row r="630">
-      <c r="E630" s="7"/>
+      <c r="F630" s="8"/>
     </row>
     <row r="631">
-      <c r="E631" s="7"/>
+      <c r="F631" s="8"/>
     </row>
     <row r="632">
-      <c r="E632" s="7"/>
+      <c r="F632" s="8"/>
     </row>
     <row r="633">
-      <c r="E633" s="7"/>
+      <c r="F633" s="8"/>
     </row>
     <row r="634">
-      <c r="E634" s="7"/>
+      <c r="F634" s="8"/>
     </row>
     <row r="635">
-      <c r="E635" s="7"/>
+      <c r="F635" s="8"/>
     </row>
     <row r="636">
-      <c r="E636" s="7"/>
+      <c r="F636" s="8"/>
     </row>
     <row r="637">
-      <c r="E637" s="7"/>
+      <c r="F637" s="8"/>
     </row>
     <row r="638">
-      <c r="E638" s="7"/>
+      <c r="F638" s="8"/>
     </row>
     <row r="639">
-      <c r="E639" s="7"/>
+      <c r="F639" s="8"/>
     </row>
     <row r="640">
-      <c r="E640" s="7"/>
+      <c r="F640" s="8"/>
     </row>
     <row r="641">
-      <c r="E641" s="7"/>
+      <c r="F641" s="8"/>
     </row>
     <row r="642">
-      <c r="E642" s="7"/>
+      <c r="F642" s="8"/>
     </row>
     <row r="643">
-      <c r="E643" s="7"/>
+      <c r="F643" s="8"/>
     </row>
     <row r="644">
-      <c r="E644" s="7"/>
+      <c r="F644" s="8"/>
     </row>
     <row r="645">
-      <c r="E645" s="7"/>
+      <c r="F645" s="8"/>
     </row>
     <row r="646">
-      <c r="E646" s="7"/>
+      <c r="F646" s="8"/>
     </row>
     <row r="647">
-      <c r="E647" s="7"/>
+      <c r="F647" s="8"/>
     </row>
     <row r="648">
-      <c r="E648" s="7"/>
+      <c r="F648" s="8"/>
     </row>
     <row r="649">
-      <c r="E649" s="7"/>
+      <c r="F649" s="8"/>
     </row>
     <row r="650">
-      <c r="E650" s="7"/>
+      <c r="F650" s="8"/>
     </row>
     <row r="651">
-      <c r="E651" s="7"/>
+      <c r="F651" s="8"/>
     </row>
     <row r="652">
-      <c r="E652" s="7"/>
+      <c r="F652" s="8"/>
     </row>
     <row r="653">
-      <c r="E653" s="7"/>
+      <c r="F653" s="8"/>
     </row>
     <row r="654">
-      <c r="E654" s="7"/>
+      <c r="F654" s="8"/>
     </row>
     <row r="655">
-      <c r="E655" s="7"/>
+      <c r="F655" s="8"/>
     </row>
     <row r="656">
-      <c r="E656" s="7"/>
+      <c r="F656" s="8"/>
     </row>
     <row r="657">
-      <c r="E657" s="7"/>
+      <c r="F657" s="8"/>
     </row>
     <row r="658">
-      <c r="E658" s="7"/>
+      <c r="F658" s="8"/>
     </row>
     <row r="659">
-      <c r="E659" s="7"/>
+      <c r="F659" s="8"/>
     </row>
     <row r="660">
-      <c r="E660" s="7"/>
+      <c r="F660" s="8"/>
     </row>
     <row r="661">
-      <c r="E661" s="7"/>
+      <c r="F661" s="8"/>
     </row>
     <row r="662">
-      <c r="E662" s="7"/>
+      <c r="F662" s="8"/>
     </row>
     <row r="663">
-      <c r="E663" s="7"/>
+      <c r="F663" s="8"/>
     </row>
     <row r="664">
-      <c r="E664" s="7"/>
+      <c r="F664" s="8"/>
     </row>
     <row r="665">
-      <c r="E665" s="7"/>
+      <c r="F665" s="8"/>
     </row>
     <row r="666">
-      <c r="E666" s="7"/>
+      <c r="F666" s="8"/>
     </row>
     <row r="667">
-      <c r="E667" s="7"/>
+      <c r="F667" s="8"/>
     </row>
     <row r="668">
-      <c r="E668" s="7"/>
+      <c r="F668" s="8"/>
     </row>
     <row r="669">
-      <c r="E669" s="7"/>
+      <c r="F669" s="8"/>
     </row>
     <row r="670">
-      <c r="E670" s="7"/>
+      <c r="F670" s="8"/>
     </row>
     <row r="671">
-      <c r="E671" s="7"/>
+      <c r="F671" s="8"/>
     </row>
     <row r="672">
-      <c r="E672" s="7"/>
+      <c r="F672" s="8"/>
     </row>
     <row r="673">
-      <c r="E673" s="7"/>
+      <c r="F673" s="8"/>
     </row>
     <row r="674">
-      <c r="E674" s="7"/>
+      <c r="F674" s="8"/>
     </row>
     <row r="675">
-      <c r="E675" s="7"/>
+      <c r="F675" s="8"/>
     </row>
     <row r="676">
-      <c r="E676" s="7"/>
+      <c r="F676" s="8"/>
     </row>
     <row r="677">
-      <c r="E677" s="7"/>
+      <c r="F677" s="8"/>
     </row>
     <row r="678">
-      <c r="E678" s="7"/>
+      <c r="F678" s="8"/>
     </row>
     <row r="679">
-      <c r="E679" s="7"/>
+      <c r="F679" s="8"/>
     </row>
     <row r="680">
-      <c r="E680" s="7"/>
+      <c r="F680" s="8"/>
     </row>
     <row r="681">
-      <c r="E681" s="7"/>
+      <c r="F681" s="8"/>
     </row>
     <row r="682">
-      <c r="E682" s="7"/>
+      <c r="F682" s="8"/>
     </row>
     <row r="683">
-      <c r="E683" s="7"/>
+      <c r="F683" s="8"/>
     </row>
     <row r="684">
-      <c r="E684" s="7"/>
+      <c r="F684" s="8"/>
     </row>
     <row r="685">
-      <c r="E685" s="7"/>
+      <c r="F685" s="8"/>
     </row>
     <row r="686">
-      <c r="E686" s="7"/>
+      <c r="F686" s="8"/>
     </row>
     <row r="687">
-      <c r="E687" s="7"/>
+      <c r="F687" s="8"/>
     </row>
     <row r="688">
-      <c r="E688" s="7"/>
+      <c r="F688" s="8"/>
     </row>
     <row r="689">
-      <c r="E689" s="7"/>
+      <c r="F689" s="8"/>
     </row>
     <row r="690">
-      <c r="E690" s="7"/>
+      <c r="F690" s="8"/>
     </row>
     <row r="691">
-      <c r="E691" s="7"/>
+      <c r="F691" s="8"/>
     </row>
     <row r="692">
-      <c r="E692" s="7"/>
+      <c r="F692" s="8"/>
     </row>
     <row r="693">
-      <c r="E693" s="7"/>
+      <c r="F693" s="8"/>
     </row>
     <row r="694">
-      <c r="E694" s="7"/>
+      <c r="F694" s="8"/>
     </row>
     <row r="695">
-      <c r="E695" s="7"/>
+      <c r="F695" s="8"/>
     </row>
     <row r="696">
-      <c r="E696" s="7"/>
+      <c r="F696" s="8"/>
     </row>
     <row r="697">
-      <c r="E697" s="7"/>
+      <c r="F697" s="8"/>
     </row>
     <row r="698">
-      <c r="E698" s="7"/>
+      <c r="F698" s="8"/>
     </row>
     <row r="699">
-      <c r="E699" s="7"/>
+      <c r="F699" s="8"/>
     </row>
     <row r="700">
-      <c r="E700" s="7"/>
+      <c r="F700" s="8"/>
     </row>
     <row r="701">
-      <c r="E701" s="7"/>
+      <c r="F701" s="8"/>
     </row>
     <row r="702">
-      <c r="E702" s="7"/>
+      <c r="F702" s="8"/>
     </row>
     <row r="703">
-      <c r="E703" s="7"/>
+      <c r="F703" s="8"/>
     </row>
     <row r="704">
-      <c r="E704" s="7"/>
+      <c r="F704" s="8"/>
     </row>
     <row r="705">
-      <c r="E705" s="7"/>
+      <c r="F705" s="8"/>
     </row>
     <row r="706">
-      <c r="E706" s="7"/>
+      <c r="F706" s="8"/>
     </row>
     <row r="707">
-      <c r="E707" s="7"/>
+      <c r="F707" s="8"/>
     </row>
     <row r="708">
-      <c r="E708" s="7"/>
+      <c r="F708" s="8"/>
     </row>
     <row r="709">
-      <c r="E709" s="7"/>
+      <c r="F709" s="8"/>
     </row>
     <row r="710">
-      <c r="E710" s="7"/>
+      <c r="F710" s="8"/>
     </row>
     <row r="711">
-      <c r="E711" s="7"/>
+      <c r="F711" s="8"/>
     </row>
     <row r="712">
-      <c r="E712" s="7"/>
+      <c r="F712" s="8"/>
     </row>
     <row r="713">
-      <c r="E713" s="7"/>
+      <c r="F713" s="8"/>
     </row>
     <row r="714">
-      <c r="E714" s="7"/>
+      <c r="F714" s="8"/>
     </row>
     <row r="715">
-      <c r="E715" s="7"/>
+      <c r="F715" s="8"/>
     </row>
     <row r="716">
-      <c r="E716" s="7"/>
+      <c r="F716" s="8"/>
     </row>
     <row r="717">
-      <c r="E717" s="7"/>
+      <c r="F717" s="8"/>
     </row>
     <row r="718">
-      <c r="E718" s="7"/>
+      <c r="F718" s="8"/>
     </row>
     <row r="719">
-      <c r="E719" s="7"/>
+      <c r="F719" s="8"/>
     </row>
     <row r="720">
-      <c r="E720" s="7"/>
+      <c r="F720" s="8"/>
     </row>
     <row r="721">
-      <c r="E721" s="7"/>
+      <c r="F721" s="8"/>
     </row>
     <row r="722">
-      <c r="E722" s="7"/>
+      <c r="F722" s="8"/>
     </row>
     <row r="723">
-      <c r="E723" s="7"/>
+      <c r="F723" s="8"/>
     </row>
     <row r="724">
-      <c r="E724" s="7"/>
+      <c r="F724" s="8"/>
     </row>
     <row r="725">
-      <c r="E725" s="7"/>
+      <c r="F725" s="8"/>
     </row>
     <row r="726">
-      <c r="E726" s="7"/>
+      <c r="F726" s="8"/>
     </row>
     <row r="727">
-      <c r="E727" s="7"/>
+      <c r="F727" s="8"/>
     </row>
     <row r="728">
-      <c r="E728" s="7"/>
+      <c r="F728" s="8"/>
     </row>
     <row r="729">
-      <c r="E729" s="7"/>
+      <c r="F729" s="8"/>
     </row>
     <row r="730">
-      <c r="E730" s="7"/>
+      <c r="F730" s="8"/>
     </row>
     <row r="731">
-      <c r="E731" s="7"/>
+      <c r="F731" s="8"/>
     </row>
     <row r="732">
-      <c r="E732" s="7"/>
+      <c r="F732" s="8"/>
     </row>
     <row r="733">
-      <c r="E733" s="7"/>
+      <c r="F733" s="8"/>
     </row>
     <row r="734">
-      <c r="E734" s="7"/>
+      <c r="F734" s="8"/>
     </row>
     <row r="735">
-      <c r="E735" s="7"/>
+      <c r="F735" s="8"/>
     </row>
     <row r="736">
-      <c r="E736" s="7"/>
+      <c r="F736" s="8"/>
     </row>
     <row r="737">
-      <c r="E737" s="7"/>
+      <c r="F737" s="8"/>
     </row>
     <row r="738">
-      <c r="E738" s="7"/>
+      <c r="F738" s="8"/>
     </row>
     <row r="739">
-      <c r="E739" s="7"/>
+      <c r="F739" s="8"/>
     </row>
     <row r="740">
-      <c r="E740" s="7"/>
+      <c r="F740" s="8"/>
     </row>
     <row r="741">
-      <c r="E741" s="7"/>
+      <c r="F741" s="8"/>
     </row>
     <row r="742">
-      <c r="E742" s="7"/>
+      <c r="F742" s="8"/>
     </row>
     <row r="743">
-      <c r="E743" s="7"/>
+      <c r="F743" s="8"/>
     </row>
     <row r="744">
-      <c r="E744" s="7"/>
+      <c r="F744" s="8"/>
     </row>
     <row r="745">
-      <c r="E745" s="7"/>
+      <c r="F745" s="8"/>
     </row>
     <row r="746">
-      <c r="E746" s="7"/>
+      <c r="F746" s="8"/>
     </row>
     <row r="747">
-      <c r="E747" s="7"/>
+      <c r="F747" s="8"/>
     </row>
     <row r="748">
-      <c r="E748" s="7"/>
+      <c r="F748" s="8"/>
     </row>
     <row r="749">
-      <c r="E749" s="7"/>
+      <c r="F749" s="8"/>
     </row>
     <row r="750">
-      <c r="E750" s="7"/>
+      <c r="F750" s="8"/>
     </row>
     <row r="751">
-      <c r="E751" s="7"/>
+      <c r="F751" s="8"/>
     </row>
     <row r="752">
-      <c r="E752" s="7"/>
+      <c r="F752" s="8"/>
     </row>
     <row r="753">
-      <c r="E753" s="7"/>
+      <c r="F753" s="8"/>
     </row>
     <row r="754">
-      <c r="E754" s="7"/>
+      <c r="F754" s="8"/>
     </row>
     <row r="755">
-      <c r="E755" s="7"/>
+      <c r="F755" s="8"/>
     </row>
     <row r="756">
-      <c r="E756" s="7"/>
+      <c r="F756" s="8"/>
     </row>
     <row r="757">
-      <c r="E757" s="7"/>
+      <c r="F757" s="8"/>
     </row>
     <row r="758">
-      <c r="E758" s="7"/>
+      <c r="F758" s="8"/>
     </row>
     <row r="759">
-      <c r="E759" s="7"/>
+      <c r="F759" s="8"/>
     </row>
     <row r="760">
-      <c r="E760" s="7"/>
+      <c r="F760" s="8"/>
     </row>
     <row r="761">
-      <c r="E761" s="7"/>
+      <c r="F761" s="8"/>
     </row>
     <row r="762">
-      <c r="E762" s="7"/>
+      <c r="F762" s="8"/>
     </row>
     <row r="763">
-      <c r="E763" s="7"/>
+      <c r="F763" s="8"/>
     </row>
     <row r="764">
-      <c r="E764" s="7"/>
+      <c r="F764" s="8"/>
     </row>
     <row r="765">
-      <c r="E765" s="7"/>
+      <c r="F765" s="8"/>
     </row>
     <row r="766">
-      <c r="E766" s="7"/>
+      <c r="F766" s="8"/>
     </row>
     <row r="767">
-      <c r="E767" s="7"/>
+      <c r="F767" s="8"/>
     </row>
     <row r="768">
-      <c r="E768" s="7"/>
+      <c r="F768" s="8"/>
     </row>
     <row r="769">
-      <c r="E769" s="7"/>
+      <c r="F769" s="8"/>
     </row>
     <row r="770">
-      <c r="E770" s="7"/>
+      <c r="F770" s="8"/>
     </row>
     <row r="771">
-      <c r="E771" s="7"/>
+      <c r="F771" s="8"/>
     </row>
     <row r="772">
-      <c r="E772" s="7"/>
+      <c r="F772" s="8"/>
     </row>
     <row r="773">
-      <c r="E773" s="7"/>
+      <c r="F773" s="8"/>
     </row>
     <row r="774">
-      <c r="E774" s="7"/>
+      <c r="F774" s="8"/>
     </row>
     <row r="775">
-      <c r="E775" s="7"/>
+      <c r="F775" s="8"/>
     </row>
     <row r="776">
-      <c r="E776" s="7"/>
+      <c r="F776" s="8"/>
     </row>
     <row r="777">
-      <c r="E777" s="7"/>
+      <c r="F777" s="8"/>
     </row>
     <row r="778">
-      <c r="E778" s="7"/>
+      <c r="F778" s="8"/>
     </row>
     <row r="779">
-      <c r="E779" s="7"/>
+      <c r="F779" s="8"/>
     </row>
     <row r="780">
-      <c r="E780" s="7"/>
+      <c r="F780" s="8"/>
     </row>
     <row r="781">
-      <c r="E781" s="7"/>
+      <c r="F781" s="8"/>
     </row>
     <row r="782">
-      <c r="E782" s="7"/>
+      <c r="F782" s="8"/>
     </row>
     <row r="783">
-      <c r="E783" s="7"/>
+      <c r="F783" s="8"/>
     </row>
     <row r="784">
-      <c r="E784" s="7"/>
+      <c r="F784" s="8"/>
     </row>
     <row r="785">
-      <c r="E785" s="7"/>
+      <c r="F785" s="8"/>
     </row>
     <row r="786">
-      <c r="E786" s="7"/>
+      <c r="F786" s="8"/>
     </row>
     <row r="787">
-      <c r="E787" s="7"/>
+      <c r="F787" s="8"/>
     </row>
     <row r="788">
-      <c r="E788" s="7"/>
+      <c r="F788" s="8"/>
     </row>
     <row r="789">
-      <c r="E789" s="7"/>
+      <c r="F789" s="8"/>
     </row>
     <row r="790">
-      <c r="E790" s="7"/>
+      <c r="F790" s="8"/>
     </row>
     <row r="791">
-      <c r="E791" s="7"/>
+      <c r="F791" s="8"/>
     </row>
     <row r="792">
-      <c r="E792" s="7"/>
+      <c r="F792" s="8"/>
     </row>
     <row r="793">
-      <c r="E793" s="7"/>
+      <c r="F793" s="8"/>
     </row>
     <row r="794">
-      <c r="E794" s="7"/>
+      <c r="F794" s="8"/>
     </row>
     <row r="795">
-      <c r="E795" s="7"/>
+      <c r="F795" s="8"/>
     </row>
     <row r="796">
-      <c r="E796" s="7"/>
+      <c r="F796" s="8"/>
     </row>
     <row r="797">
-      <c r="E797" s="7"/>
+      <c r="F797" s="8"/>
     </row>
     <row r="798">
-      <c r="E798" s="7"/>
+      <c r="F798" s="8"/>
     </row>
     <row r="799">
-      <c r="E799" s="7"/>
+      <c r="F799" s="8"/>
     </row>
     <row r="800">
-      <c r="E800" s="7"/>
+      <c r="F800" s="8"/>
     </row>
     <row r="801">
-      <c r="E801" s="7"/>
+      <c r="F801" s="8"/>
     </row>
     <row r="802">
-      <c r="E802" s="7"/>
+      <c r="F802" s="8"/>
     </row>
     <row r="803">
-      <c r="E803" s="7"/>
+      <c r="F803" s="8"/>
     </row>
     <row r="804">
-      <c r="E804" s="7"/>
+      <c r="F804" s="8"/>
     </row>
     <row r="805">
-      <c r="E805" s="7"/>
+      <c r="F805" s="8"/>
     </row>
     <row r="806">
-      <c r="E806" s="7"/>
+      <c r="F806" s="8"/>
     </row>
     <row r="807">
-      <c r="E807" s="7"/>
+      <c r="F807" s="8"/>
     </row>
     <row r="808">
-      <c r="E808" s="7"/>
+      <c r="F808" s="8"/>
     </row>
     <row r="809">
-      <c r="E809" s="7"/>
+      <c r="F809" s="8"/>
     </row>
     <row r="810">
-      <c r="E810" s="7"/>
+      <c r="F810" s="8"/>
     </row>
     <row r="811">
-      <c r="E811" s="7"/>
+      <c r="F811" s="8"/>
     </row>
     <row r="812">
-      <c r="E812" s="7"/>
+      <c r="F812" s="8"/>
     </row>
     <row r="813">
-      <c r="E813" s="7"/>
+      <c r="F813" s="8"/>
     </row>
     <row r="814">
-      <c r="E814" s="7"/>
+      <c r="F814" s="8"/>
     </row>
     <row r="815">
-      <c r="E815" s="7"/>
+      <c r="F815" s="8"/>
     </row>
     <row r="816">
-      <c r="E816" s="7"/>
+      <c r="F816" s="8"/>
     </row>
     <row r="817">
-      <c r="E817" s="7"/>
+      <c r="F817" s="8"/>
     </row>
     <row r="818">
-      <c r="E818" s="7"/>
+      <c r="F818" s="8"/>
     </row>
     <row r="819">
-      <c r="E819" s="7"/>
+      <c r="F819" s="8"/>
     </row>
     <row r="820">
-      <c r="E820" s="7"/>
+      <c r="F820" s="8"/>
     </row>
     <row r="821">
-      <c r="E821" s="7"/>
+      <c r="F821" s="8"/>
     </row>
     <row r="822">
-      <c r="E822" s="7"/>
+      <c r="F822" s="8"/>
     </row>
     <row r="823">
-      <c r="E823" s="7"/>
+      <c r="F823" s="8"/>
     </row>
     <row r="824">
-      <c r="E824" s="7"/>
+      <c r="F824" s="8"/>
     </row>
     <row r="825">
-      <c r="E825" s="7"/>
+      <c r="F825" s="8"/>
     </row>
     <row r="826">
-      <c r="E826" s="7"/>
+      <c r="F826" s="8"/>
     </row>
     <row r="827">
-      <c r="E827" s="7"/>
+      <c r="F827" s="8"/>
     </row>
     <row r="828">
-      <c r="E828" s="7"/>
+      <c r="F828" s="8"/>
     </row>
     <row r="829">
-      <c r="E829" s="7"/>
+      <c r="F829" s="8"/>
     </row>
     <row r="830">
-      <c r="E830" s="7"/>
+      <c r="F830" s="8"/>
     </row>
     <row r="831">
-      <c r="E831" s="7"/>
+      <c r="F831" s="8"/>
     </row>
     <row r="832">
-      <c r="E832" s="7"/>
+      <c r="F832" s="8"/>
     </row>
     <row r="833">
-      <c r="E833" s="7"/>
+      <c r="F833" s="8"/>
     </row>
     <row r="834">
-      <c r="E834" s="7"/>
+      <c r="F834" s="8"/>
     </row>
     <row r="835">
-      <c r="E835" s="7"/>
+      <c r="F835" s="8"/>
     </row>
     <row r="836">
-      <c r="E836" s="7"/>
+      <c r="F836" s="8"/>
     </row>
     <row r="837">
-      <c r="E837" s="7"/>
+      <c r="F837" s="8"/>
     </row>
     <row r="838">
-      <c r="E838" s="7"/>
+      <c r="F838" s="8"/>
     </row>
     <row r="839">
-      <c r="E839" s="7"/>
+      <c r="F839" s="8"/>
     </row>
     <row r="840">
-      <c r="E840" s="7"/>
+      <c r="F840" s="8"/>
     </row>
     <row r="841">
-      <c r="E841" s="7"/>
+      <c r="F841" s="8"/>
     </row>
     <row r="842">
-      <c r="E842" s="7"/>
+      <c r="F842" s="8"/>
     </row>
     <row r="843">
-      <c r="E843" s="7"/>
+      <c r="F843" s="8"/>
     </row>
     <row r="844">
-      <c r="E844" s="7"/>
+      <c r="F844" s="8"/>
     </row>
     <row r="845">
-      <c r="E845" s="7"/>
+      <c r="F845" s="8"/>
     </row>
     <row r="846">
-      <c r="E846" s="7"/>
+      <c r="F846" s="8"/>
     </row>
     <row r="847">
-      <c r="E847" s="7"/>
+      <c r="F847" s="8"/>
     </row>
     <row r="848">
-      <c r="E848" s="7"/>
+      <c r="F848" s="8"/>
     </row>
     <row r="849">
-      <c r="E849" s="7"/>
+      <c r="F849" s="8"/>
     </row>
     <row r="850">
-      <c r="E850" s="7"/>
+      <c r="F850" s="8"/>
     </row>
     <row r="851">
-      <c r="E851" s="7"/>
+      <c r="F851" s="8"/>
     </row>
     <row r="852">
-      <c r="E852" s="7"/>
+      <c r="F852" s="8"/>
     </row>
     <row r="853">
-      <c r="E853" s="7"/>
+      <c r="F853" s="8"/>
     </row>
     <row r="854">
-      <c r="E854" s="7"/>
+      <c r="F854" s="8"/>
     </row>
     <row r="855">
-      <c r="E855" s="7"/>
+      <c r="F855" s="8"/>
     </row>
     <row r="856">
-      <c r="E856" s="7"/>
+      <c r="F856" s="8"/>
     </row>
     <row r="857">
-      <c r="E857" s="7"/>
+      <c r="F857" s="8"/>
     </row>
     <row r="858">
-      <c r="E858" s="7"/>
+      <c r="F858" s="8"/>
     </row>
     <row r="859">
-      <c r="E859" s="7"/>
+      <c r="F859" s="8"/>
     </row>
     <row r="860">
-      <c r="E860" s="7"/>
+      <c r="F860" s="8"/>
     </row>
     <row r="861">
-      <c r="E861" s="7"/>
+      <c r="F861" s="8"/>
     </row>
     <row r="862">
-      <c r="E862" s="7"/>
+      <c r="F862" s="8"/>
     </row>
     <row r="863">
-      <c r="E863" s="7"/>
+      <c r="F863" s="8"/>
     </row>
     <row r="864">
-      <c r="E864" s="7"/>
+      <c r="F864" s="8"/>
     </row>
     <row r="865">
-      <c r="E865" s="7"/>
+      <c r="F865" s="8"/>
     </row>
     <row r="866">
-      <c r="E866" s="7"/>
+      <c r="F866" s="8"/>
     </row>
     <row r="867">
-      <c r="E867" s="7"/>
+      <c r="F867" s="8"/>
     </row>
     <row r="868">
-      <c r="E868" s="7"/>
+      <c r="F868" s="8"/>
     </row>
     <row r="869">
-      <c r="E869" s="7"/>
+      <c r="F869" s="8"/>
     </row>
     <row r="870">
-      <c r="E870" s="7"/>
+      <c r="F870" s="8"/>
     </row>
     <row r="871">
-      <c r="E871" s="7"/>
+      <c r="F871" s="8"/>
     </row>
     <row r="872">
-      <c r="E872" s="7"/>
+      <c r="F872" s="8"/>
     </row>
     <row r="873">
-      <c r="E873" s="7"/>
+      <c r="F873" s="8"/>
     </row>
     <row r="874">
-      <c r="E874" s="7"/>
+      <c r="F874" s="8"/>
     </row>
     <row r="875">
-      <c r="E875" s="7"/>
+      <c r="F875" s="8"/>
     </row>
     <row r="876">
-      <c r="E876" s="7"/>
+      <c r="F876" s="8"/>
     </row>
     <row r="877">
-      <c r="E877" s="7"/>
+      <c r="F877" s="8"/>
     </row>
     <row r="878">
-      <c r="E878" s="7"/>
+      <c r="F878" s="8"/>
     </row>
     <row r="879">
-      <c r="E879" s="7"/>
+      <c r="F879" s="8"/>
     </row>
     <row r="880">
-      <c r="E880" s="7"/>
+      <c r="F880" s="8"/>
     </row>
     <row r="881">
-      <c r="E881" s="7"/>
+      <c r="F881" s="8"/>
     </row>
     <row r="882">
-      <c r="E882" s="7"/>
+      <c r="F882" s="8"/>
     </row>
     <row r="883">
-      <c r="E883" s="7"/>
+      <c r="F883" s="8"/>
     </row>
     <row r="884">
-      <c r="E884" s="7"/>
+      <c r="F884" s="8"/>
     </row>
     <row r="885">
-      <c r="E885" s="7"/>
+      <c r="F885" s="8"/>
     </row>
     <row r="886">
-      <c r="E886" s="7"/>
+      <c r="F886" s="8"/>
     </row>
     <row r="887">
-      <c r="E887" s="7"/>
+      <c r="F887" s="8"/>
     </row>
     <row r="888">
-      <c r="E888" s="7"/>
+      <c r="F888" s="8"/>
     </row>
     <row r="889">
-      <c r="E889" s="7"/>
+      <c r="F889" s="8"/>
     </row>
     <row r="890">
-      <c r="E890" s="7"/>
+      <c r="F890" s="8"/>
     </row>
     <row r="891">
-      <c r="E891" s="7"/>
+      <c r="F891" s="8"/>
     </row>
     <row r="892">
-      <c r="E892" s="7"/>
+      <c r="F892" s="8"/>
     </row>
     <row r="893">
-      <c r="E893" s="7"/>
+      <c r="F893" s="8"/>
     </row>
     <row r="894">
-      <c r="E894" s="7"/>
+      <c r="F894" s="8"/>
     </row>
     <row r="895">
-      <c r="E895" s="7"/>
+      <c r="F895" s="8"/>
     </row>
     <row r="896">
-      <c r="E896" s="7"/>
+      <c r="F896" s="8"/>
     </row>
     <row r="897">
-      <c r="E897" s="7"/>
+      <c r="F897" s="8"/>
     </row>
     <row r="898">
-      <c r="E898" s="7"/>
+      <c r="F898" s="8"/>
     </row>
     <row r="899">
-      <c r="E899" s="7"/>
+      <c r="F899" s="8"/>
     </row>
     <row r="900">
-      <c r="E900" s="7"/>
+      <c r="F900" s="8"/>
     </row>
     <row r="901">
-      <c r="E901" s="7"/>
+      <c r="F901" s="8"/>
     </row>
     <row r="902">
-      <c r="E902" s="7"/>
+      <c r="F902" s="8"/>
     </row>
     <row r="903">
-      <c r="E903" s="7"/>
+      <c r="F903" s="8"/>
     </row>
     <row r="904">
-      <c r="E904" s="7"/>
+      <c r="F904" s="8"/>
     </row>
     <row r="905">
-      <c r="E905" s="7"/>
+      <c r="F905" s="8"/>
     </row>
     <row r="906">
-      <c r="E906" s="7"/>
+      <c r="F906" s="8"/>
     </row>
     <row r="907">
-      <c r="E907" s="7"/>
+      <c r="F907" s="8"/>
     </row>
     <row r="908">
-      <c r="E908" s="7"/>
+      <c r="F908" s="8"/>
     </row>
     <row r="909">
-      <c r="E909" s="7"/>
+      <c r="F909" s="8"/>
     </row>
     <row r="910">
-      <c r="E910" s="7"/>
+      <c r="F910" s="8"/>
     </row>
     <row r="911">
-      <c r="E911" s="7"/>
+      <c r="F911" s="8"/>
     </row>
     <row r="912">
-      <c r="E912" s="7"/>
+      <c r="F912" s="8"/>
     </row>
     <row r="913">
-      <c r="E913" s="7"/>
+      <c r="F913" s="8"/>
     </row>
     <row r="914">
-      <c r="E914" s="7"/>
+      <c r="F914" s="8"/>
     </row>
     <row r="915">
-      <c r="E915" s="7"/>
+      <c r="F915" s="8"/>
     </row>
     <row r="916">
-      <c r="E916" s="7"/>
+      <c r="F916" s="8"/>
     </row>
     <row r="917">
-      <c r="E917" s="7"/>
+      <c r="F917" s="8"/>
     </row>
     <row r="918">
-      <c r="E918" s="7"/>
+      <c r="F918" s="8"/>
     </row>
     <row r="919">
-      <c r="E919" s="7"/>
+      <c r="F919" s="8"/>
     </row>
     <row r="920">
-      <c r="E920" s="7"/>
+      <c r="F920" s="8"/>
     </row>
     <row r="921">
-      <c r="E921" s="7"/>
+      <c r="F921" s="8"/>
     </row>
     <row r="922">
-      <c r="E922" s="7"/>
+      <c r="F922" s="8"/>
     </row>
     <row r="923">
-      <c r="E923" s="7"/>
+      <c r="F923" s="8"/>
     </row>
     <row r="924">
-      <c r="E924" s="7"/>
+      <c r="F924" s="8"/>
     </row>
     <row r="925">
-      <c r="E925" s="7"/>
+      <c r="F925" s="8"/>
     </row>
     <row r="926">
-      <c r="E926" s="7"/>
+      <c r="F926" s="8"/>
     </row>
     <row r="927">
-      <c r="E927" s="7"/>
+      <c r="F927" s="8"/>
     </row>
     <row r="928">
-      <c r="E928" s="7"/>
+      <c r="F928" s="8"/>
     </row>
     <row r="929">
-      <c r="E929" s="7"/>
+      <c r="F929" s="8"/>
     </row>
     <row r="930">
-      <c r="E930" s="7"/>
+      <c r="F930" s="8"/>
     </row>
     <row r="931">
-      <c r="E931" s="7"/>
+      <c r="F931" s="8"/>
     </row>
     <row r="932">
-      <c r="E932" s="7"/>
+      <c r="F932" s="8"/>
     </row>
     <row r="933">
-      <c r="E933" s="7"/>
+      <c r="F933" s="8"/>
     </row>
     <row r="934">
-      <c r="E934" s="7"/>
+      <c r="F934" s="8"/>
     </row>
     <row r="935">
-      <c r="E935" s="7"/>
+      <c r="F935" s="8"/>
     </row>
     <row r="936">
-      <c r="E936" s="7"/>
+      <c r="F936" s="8"/>
     </row>
     <row r="937">
-      <c r="E937" s="7"/>
+      <c r="F937" s="8"/>
     </row>
     <row r="938">
-      <c r="E938" s="7"/>
+      <c r="F938" s="8"/>
     </row>
     <row r="939">
-      <c r="E939" s="7"/>
+      <c r="F939" s="8"/>
     </row>
     <row r="940">
-      <c r="E940" s="7"/>
+      <c r="F940" s="8"/>
     </row>
     <row r="941">
-      <c r="E941" s="7"/>
+      <c r="F941" s="8"/>
     </row>
     <row r="942">
-      <c r="E942" s="7"/>
+      <c r="F942" s="8"/>
     </row>
     <row r="943">
-      <c r="E943" s="7"/>
+      <c r="F943" s="8"/>
     </row>
     <row r="944">
-      <c r="E944" s="7"/>
+      <c r="F944" s="8"/>
     </row>
     <row r="945">
-      <c r="E945" s="7"/>
+      <c r="F945" s="8"/>
     </row>
     <row r="946">
-      <c r="E946" s="7"/>
+      <c r="F946" s="8"/>
     </row>
     <row r="947">
-      <c r="E947" s="7"/>
+      <c r="F947" s="8"/>
     </row>
     <row r="948">
-      <c r="E948" s="7"/>
+      <c r="F948" s="8"/>
     </row>
     <row r="949">
-      <c r="E949" s="7"/>
+      <c r="F949" s="8"/>
     </row>
     <row r="950">
-      <c r="E950" s="7"/>
+      <c r="F950" s="8"/>
     </row>
     <row r="951">
-      <c r="E951" s="7"/>
+      <c r="F951" s="8"/>
     </row>
     <row r="952">
-      <c r="E952" s="7"/>
+      <c r="F952" s="8"/>
     </row>
     <row r="953">
-      <c r="E953" s="7"/>
+      <c r="F953" s="8"/>
     </row>
     <row r="954">
-      <c r="E954" s="7"/>
+      <c r="F954" s="8"/>
     </row>
     <row r="955">
-      <c r="E955" s="7"/>
+      <c r="F955" s="8"/>
     </row>
     <row r="956">
-      <c r="E956" s="7"/>
+      <c r="F956" s="8"/>
     </row>
     <row r="957">
-      <c r="E957" s="7"/>
+      <c r="F957" s="8"/>
     </row>
     <row r="958">
-      <c r="E958" s="7"/>
+      <c r="F958" s="8"/>
     </row>
     <row r="959">
-      <c r="E959" s="7"/>
+      <c r="F959" s="8"/>
     </row>
     <row r="960">
-      <c r="E960" s="7"/>
+      <c r="F960" s="8"/>
     </row>
     <row r="961">
-      <c r="E961" s="7"/>
+      <c r="F961" s="8"/>
     </row>
     <row r="962">
-      <c r="E962" s="7"/>
+      <c r="F962" s="8"/>
     </row>
     <row r="963">
-      <c r="E963" s="7"/>
+      <c r="F963" s="8"/>
     </row>
     <row r="964">
-      <c r="E964" s="7"/>
+      <c r="F964" s="8"/>
     </row>
     <row r="965">
-      <c r="E965" s="7"/>
+      <c r="F965" s="8"/>
     </row>
     <row r="966">
-      <c r="E966" s="7"/>
+      <c r="F966" s="8"/>
     </row>
     <row r="967">
-      <c r="E967" s="7"/>
+      <c r="F967" s="8"/>
     </row>
     <row r="968">
-      <c r="E968" s="7"/>
+      <c r="F968" s="8"/>
     </row>
     <row r="969">
-      <c r="E969" s="7"/>
+      <c r="F969" s="8"/>
     </row>
     <row r="970">
-      <c r="E970" s="7"/>
+      <c r="F970" s="8"/>
     </row>
     <row r="971">
-      <c r="E971" s="7"/>
+      <c r="F971" s="8"/>
     </row>
     <row r="972">
-      <c r="E972" s="7"/>
+      <c r="F972" s="8"/>
     </row>
     <row r="973">
-      <c r="E973" s="7"/>
+      <c r="F973" s="8"/>
     </row>
     <row r="974">
-      <c r="E974" s="7"/>
+      <c r="F974" s="8"/>
     </row>
     <row r="975">
-      <c r="E975" s="7"/>
+      <c r="F975" s="8"/>
     </row>
     <row r="976">
-      <c r="E976" s="7"/>
+      <c r="F976" s="8"/>
     </row>
     <row r="977">
-      <c r="E977" s="7"/>
+      <c r="F977" s="8"/>
     </row>
     <row r="978">
-      <c r="E978" s="7"/>
+      <c r="F978" s="8"/>
     </row>
     <row r="979">
-      <c r="E979" s="7"/>
+      <c r="F979" s="8"/>
     </row>
     <row r="980">
-      <c r="E980" s="7"/>
+      <c r="F980" s="8"/>
     </row>
     <row r="981">
-      <c r="E981" s="7"/>
+      <c r="F981" s="8"/>
     </row>
     <row r="982">
-      <c r="E982" s="7"/>
+      <c r="F982" s="8"/>
     </row>
     <row r="983">
-      <c r="E983" s="7"/>
+      <c r="F983" s="8"/>
     </row>
     <row r="984">
-      <c r="E984" s="7"/>
+      <c r="F984" s="8"/>
     </row>
     <row r="985">
-      <c r="E985" s="7"/>
+      <c r="F985" s="8"/>
     </row>
     <row r="986">
-      <c r="E986" s="7"/>
+      <c r="F986" s="8"/>
     </row>
     <row r="987">
-      <c r="E987" s="7"/>
+      <c r="F987" s="8"/>
     </row>
     <row r="988">
-      <c r="E988" s="7"/>
+      <c r="F988" s="8"/>
     </row>
     <row r="989">
-      <c r="E989" s="7"/>
+      <c r="F989" s="8"/>
     </row>
     <row r="990">
-      <c r="E990" s="7"/>
+      <c r="F990" s="8"/>
     </row>
     <row r="991">
-      <c r="E991" s="7"/>
+      <c r="F991" s="8"/>
     </row>
     <row r="992">
-      <c r="E992" s="7"/>
+      <c r="F992" s="8"/>
     </row>
     <row r="993">
-      <c r="E993" s="7"/>
+      <c r="F993" s="8"/>
     </row>
     <row r="994">
-      <c r="E994" s="7"/>
+      <c r="F994" s="8"/>
     </row>
     <row r="995">
-      <c r="E995" s="7"/>
+      <c r="F995" s="8"/>
     </row>
     <row r="996">
-      <c r="E996" s="7"/>
+      <c r="F996" s="8"/>
     </row>
     <row r="997">
-      <c r="E997" s="7"/>
+      <c r="F997" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3932,6 +3975,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="19.13"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -3946,35 +3992,35 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1">
         <v>200.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>404.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
         <v>404.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added changes to validate no auth feature
</commit_message>
<xml_diff>
--- a/src/test/resources/swagger-testData.xlsx
+++ b/src/test/resources/swagger-testData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="118">
   <si>
     <t>scenario</t>
   </si>
@@ -83,6 +83,15 @@
     <t>Not Found</t>
   </si>
   <si>
+    <t>noAuth</t>
+  </si>
+  <si>
+    <t>HTTP/1.1 401 Unauthorized</t>
+  </si>
+  <si>
+    <t>Unauthorized</t>
+  </si>
+  <si>
     <t>userFirstName</t>
   </si>
   <si>
@@ -263,6 +272,12 @@
     <t>Plot number should contain alphaNumeric values only</t>
   </si>
   <si>
+    <t>february</t>
+  </si>
+  <si>
+    <t>Team09Sandhya38@gmail.com</t>
+  </si>
+  <si>
     <t>/updateuser/{userId}</t>
   </si>
   <si>
@@ -278,9 +293,6 @@
     <t>plot-31</t>
   </si>
   <si>
-    <t>Team09Sandhya38@gmail.com</t>
-  </si>
-  <si>
     <t>User email Id is required</t>
   </si>
   <si>
@@ -288,9 +300,6 @@
   </si>
   <si>
     <t>/updateuser/343434434</t>
-  </si>
-  <si>
-    <t>february</t>
   </si>
   <si>
     <t>User not found with id: 343434434</t>
@@ -782,6 +791,23 @@
         <v>21</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1">
+        <v>401.0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -820,31 +846,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>4</v>
@@ -852,392 +878,432 @@
     </row>
     <row r="2" ht="41.25" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1">
         <v>201.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G2" s="6">
         <v>3.456789015E9</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M2" s="6">
         <v>94530.0</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1">
         <v>409.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G3" s="7">
         <v>1.234567891E9</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M3" s="6">
         <v>94530.0</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1">
         <v>409.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G4" s="1">
         <v>2.234560221E9</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M4" s="6">
         <v>94530.0</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" ht="21.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1">
         <v>201.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G5" s="1">
         <v>2.234560901E9</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="6"/>
       <c r="N5" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1">
         <v>400.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E6" s="9">
         <v>45909.0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G6" s="1">
         <v>2.234560921E9</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M6" s="6">
         <v>94530.0</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1">
         <v>400.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G7" s="1">
         <v>2.234560931E9</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M7" s="6">
         <v>94530.0</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B8" s="1">
         <v>400.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G8" s="1">
         <v>12.0</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M8" s="6">
         <v>94530.0</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B9" s="1">
         <v>400.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G9" s="1">
         <v>2.234560941E9</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M9" s="6">
         <v>94530.0</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B10" s="1">
         <v>400.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G10" s="1">
         <v>2.234560951E9</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M10" s="6">
         <v>94530.0</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
-      <c r="H11" s="10"/>
-      <c r="N11" s="10"/>
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1">
+        <v>401.0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2.234560951E9</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="6">
+        <v>94530.0</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12">
       <c r="H12" s="10"/>
@@ -5219,31 +5285,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>4</v>
@@ -5251,7 +5317,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1">
         <v>200.0</v>
@@ -5260,213 +5326,213 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G2" s="7">
         <v>3.456789016E9</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M2" s="7">
         <v>94531.0</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1">
         <v>409.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G3" s="7">
         <v>1.234567891E9</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M3" s="6">
         <v>94530.0</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1">
         <v>409.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G4" s="1">
         <v>2.234560221E9</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M4" s="6">
         <v>94530.0</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B5" s="1">
         <v>400.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G5" s="1">
         <v>12.0</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M5" s="6">
         <v>94530.0</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B6" s="1">
         <v>400.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G6" s="1">
         <v>2.234560931E9</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M6" s="6">
         <v>94530.0</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
@@ -5480,31 +5546,31 @@
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G7" s="1">
         <v>2.234560941E9</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M7" s="6">
         <v>94530.0</v>
@@ -5524,81 +5590,125 @@
         <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G8" s="1">
         <v>2.234560951E9</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M8" s="6">
         <v>94530.0</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B9" s="1">
         <v>400.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G9" s="1">
         <v>2.234560961E9</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M9" s="6">
         <v>94530.0</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1">
+        <v>401.0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2.234560951E9</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="6">
+        <v>94530.0</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -5636,31 +5746,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>4</v>
@@ -5668,7 +5778,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B2" s="1">
         <v>200.0</v>
@@ -5677,42 +5787,42 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G2" s="7">
         <v>3.456789016E9</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M2" s="7">
         <v>94531.0</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" ht="37.5" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B3" s="1">
         <v>200.0</v>
@@ -5721,42 +5831,42 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G3" s="7">
         <v>3.456789016E9</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M3" s="7">
         <v>94531.0</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" ht="37.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B4" s="1">
         <v>200.0</v>
@@ -5765,257 +5875,257 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G4" s="7">
         <v>3.456789016E9</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M4" s="7">
         <v>94531.0</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1">
         <v>409.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G5" s="7">
         <v>1.234567891E9</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M5" s="6">
         <v>94530.0</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1">
         <v>409.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G6" s="1">
         <v>2.234560221E9</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M6" s="6">
         <v>94530.0</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B7" s="1">
         <v>400.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G7" s="1">
         <v>12.0</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M7" s="6">
         <v>94530.0</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B8" s="1">
         <v>400.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G8" s="1">
         <v>2.234560901E9</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M8" s="6">
         <v>94530.0</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B9" s="1">
         <v>400.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G9" s="1">
         <v>2.234560901E9</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M9" s="6">
         <v>94530.0</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
@@ -6029,37 +6139,37 @@
         <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G10" s="1">
         <v>2.234560901E9</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M10" s="6">
         <v>94530.0</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11">
@@ -6073,37 +6183,81 @@
         <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G11" s="1">
         <v>2.234560901E9</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M11" s="6">
         <v>94530.0</v>
       </c>
       <c r="N11" s="5" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1">
+        <v>401.0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2.234560951E9</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="6">
+        <v>94530.0</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -6144,7 +6298,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1">
         <v>200.0</v>
@@ -6153,15 +6307,15 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B3" s="1">
         <v>200.0</v>
@@ -6170,10 +6324,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4">
@@ -6187,10 +6341,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5">
@@ -6204,10 +6358,27 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1">
+        <v>401.0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated changes for features to run independently
</commit_message>
<xml_diff>
--- a/src/test/resources/swagger-testData.xlsx
+++ b/src/test/resources/swagger-testData.xlsx
@@ -5792,17 +5792,17 @@
       <c r="E2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" s="7">
-        <v>3.456789016E9</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>91</v>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="6">
+        <v>3.456789015E9</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>41</v>
@@ -5813,8 +5813,8 @@
       <c r="L2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="7">
-        <v>94531.0</v>
+      <c r="M2" s="6">
+        <v>94530.0</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>44</v>
@@ -5836,17 +5836,17 @@
       <c r="E3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G3" s="7">
-        <v>3.456789016E9</v>
+      <c r="F3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="6">
+        <v>3.456789015E9</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>102</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>41</v>
@@ -5857,8 +5857,8 @@
       <c r="L3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M3" s="7">
-        <v>94531.0</v>
+      <c r="M3" s="6">
+        <v>94530.0</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>44</v>
@@ -5880,11 +5880,11 @@
       <c r="E4" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G4" s="7">
-        <v>3.456789016E9</v>
+      <c r="F4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="6">
+        <v>3.456789015E9</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>102</v>

</xml_diff>